<commit_message>
Se agrego el scraping de TowerOne con descarga a ubicación del proyecto del archivo y cambio de nombre
</commit_message>
<xml_diff>
--- a/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
+++ b/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU211"/>
+  <dimension ref="A1:CU212"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -591,6 +591,7 @@
     <col min="208" max="208" width="20.83203125" customWidth="1"/>
     <col min="209" max="209" width="20.83203125" customWidth="1"/>
     <col min="210" max="210" width="20.83203125" customWidth="1"/>
+    <col min="211" max="211" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1095,7 +1096,10 @@
         <v>44988</v>
       </c>
       <c r="CP2" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ2" s="1">
+        <v>44987</v>
       </c>
       <c r="CR2" t="str">
         <v>SI</v>
@@ -1604,7 +1608,10 @@
         <v>44979</v>
       </c>
       <c r="CP4" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ4" s="1">
+        <v>44987</v>
       </c>
       <c r="CR4" t="str">
         <v>SI</v>
@@ -1849,10 +1856,10 @@
         <v>44980</v>
       </c>
       <c r="CH5" t="str">
-        <v>Aprobado con Pendientes</v>
+        <v>Aprobado</v>
       </c>
       <c r="CI5" s="1">
-        <v>44991</v>
+        <v>45009</v>
       </c>
       <c r="CJ5">
         <v>20704913</v>
@@ -1895,6 +1902,7 @@
 [2023-03-09 16:21:32] (Kevin Guerrero) Fecha Entrega ATP Rf - ATP RF: SOPORTE CORREGIDO: Anexo ATP con corrección de KPIs, el Cover esta Ok. 
 [2023-03-09 16:32:56] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: ANT7036 ATP TX: Se evidencian niveles RX acordes con cálculos de Ingeniería, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK. Sitio en Operación y en seguimiento por Garantía.
 [2023-03-10 10:09:15] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: ANT7036 ATP RF: COVER OK, VSWR OK, ALARM major, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI OK. NOTA: completan Cover y agregan graficas con sitio en servicio
+[2023-03-24 11:52:51] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: COVER ok, Medición VSWR OK, SIN ALARMAS, CROSS OK, Configuración de Parámetros y validación mediante el MML Command, SERIALES OK, INSTALACION OK. Sitio en servicio
 </v>
       </c>
       <c r="CU5" t="str" xml:space="preserve">
@@ -1945,7 +1953,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O6" t="str">
         <v>3.Power</v>
@@ -1972,10 +1980,10 @@
         <v>44979</v>
       </c>
       <c r="AA6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AB6" s="1">
-        <v>45011</v>
+        <v>45015</v>
       </c>
       <c r="AC6" s="1">
         <v>44991</v>
@@ -2053,10 +2061,10 @@
         <v>READY. OC E2E 20711768</v>
       </c>
       <c r="BR6" s="1">
-        <v>45014</v>
+        <v>45018</v>
       </c>
       <c r="BZ6" s="1">
-        <v>45016</v>
+        <v>45020</v>
       </c>
       <c r="CE6" t="str">
         <v>Pendiente vendor</v>
@@ -2481,7 +2489,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O9" t="str">
         <v>1.SAQ</v>
@@ -2571,10 +2579,10 @@
         <v>READY. (20304147 OC E2E)</v>
       </c>
       <c r="BR9" s="1">
-        <v>45798</v>
+        <v>45800</v>
       </c>
       <c r="BZ9" s="1">
-        <v>45801</v>
+        <v>45803</v>
       </c>
       <c r="CE9" t="str">
         <v>Pendiente vendor</v>
@@ -2761,10 +2769,10 @@
         <v>44979</v>
       </c>
       <c r="X11" s="1">
-        <v>45012</v>
+        <v>45016</v>
       </c>
       <c r="Y11" s="1">
-        <v>45012</v>
+        <v>45016</v>
       </c>
       <c r="AA11">
         <v>16</v>
@@ -2773,7 +2781,7 @@
         <v>45026</v>
       </c>
       <c r="AC11" s="1">
-        <v>45010</v>
+        <v>45016</v>
       </c>
       <c r="AF11" s="1">
         <v>44972</v>
@@ -3167,7 +3175,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O13" t="str">
         <v>4.Instalación Tx</v>
@@ -3278,13 +3286,13 @@
         <v>44928</v>
       </c>
       <c r="BR13" s="1">
-        <v>45011</v>
+        <v>45018</v>
       </c>
       <c r="BU13" t="str">
         <v>sitio Vandalizado - Se espera recuperación en 9 días</v>
       </c>
       <c r="BZ13" s="1">
-        <v>45011</v>
+        <v>45018</v>
       </c>
       <c r="CE13" t="str">
         <v>Pendiente vendor</v>
@@ -3562,7 +3570,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N16">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O16" t="str">
         <v>4.Instalación Tx</v>
@@ -3682,13 +3690,13 @@
         <v>44977</v>
       </c>
       <c r="BR16" s="1">
-        <v>45002</v>
+        <v>45018</v>
       </c>
       <c r="BU16" t="str">
         <v>Paro Minero - NEC debe regresar a sitio</v>
       </c>
       <c r="BZ16" s="1">
-        <v>45011</v>
+        <v>45018</v>
       </c>
       <c r="CE16" t="str">
         <v>Pendiente vendor</v>
@@ -3771,10 +3779,10 @@
         <v>12</v>
       </c>
       <c r="O17" t="str">
-        <v>6.ON AIR</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P17" t="str">
-        <v>F1-OA-ON AIR</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S17" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -3926,8 +3934,20 @@
       <c r="CH17" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="CJ17">
+        <v>20727384</v>
+      </c>
+      <c r="CK17" s="1">
+        <v>45008</v>
+      </c>
+      <c r="CL17" s="1">
+        <v>45006</v>
+      </c>
       <c r="CP17" t="str">
-        <v>Sin Entregar</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ17" s="1">
+        <v>45002</v>
       </c>
       <c r="CR17" t="str">
         <v>SI</v>
@@ -3997,7 +4017,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N18">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O18" t="str">
         <v>5.Instalación RF</v>
@@ -4132,13 +4152,16 @@
         <v>44977</v>
       </c>
       <c r="BZ18" s="1">
-        <v>45011</v>
+        <v>45018</v>
       </c>
       <c r="CD18" s="1">
         <v>44992</v>
       </c>
       <c r="CE18" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CF18" s="1">
+        <v>45007</v>
       </c>
       <c r="CH18" t="str">
         <v>Pendiente vendor</v>
@@ -4165,10 +4188,11 @@
 [2023-03-06 10:00:31] (Luis Collazos) Comentarios Generales: Se espera reunión con la comunidad luego del paro minero alrededor del 8 de marzo
 [2023-03-07 12:30:09] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacon correspondiente
 [2023-03-08 10:07:55] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: ANT7063    ATP TX: NIVELES OK, Instalación OK, TH 99Mb/99Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
+[2023-03-22 15:20:05] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO:  SOPORTE APROBADO: ANT7063 ATP TX: NIVELES OK, Instalación OK, TH 99Mb/99Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 </v>
       </c>
       <c r="CU18" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/ANT7063/Instalacion_TX/ATP-TX_ANT7063_NEC_07-03-2023.zip
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/ANT7063/Instalacion_TX/ATP-TX_ANT7063_NEC_07-03-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7063/OC/RNP_ANT7063_TOWER3_22-07-2022.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7063/Tx/ANT7063_E2E-1_11-01-2023.xlsx
 </v>
@@ -4362,7 +4386,10 @@
         <v>44994</v>
       </c>
       <c r="CE19" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CF19" s="1">
+        <v>45009</v>
       </c>
       <c r="CG19" s="1">
         <v>44987</v>
@@ -4383,7 +4410,10 @@
         <v>44980</v>
       </c>
       <c r="CP19" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ19" s="1">
+        <v>44987</v>
       </c>
       <c r="CR19" t="str">
         <v>SI</v>
@@ -4411,11 +4441,12 @@
 [2023-03-09 10:20:06] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacion correspondiente
 [2023-03-09 17:58:55] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: ANT7136    ATP TX: NIVELES OK, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 [2023-03-10 09:55:34] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: COVER OK, VSWR OK, Sin Alarmas presentes, SERIALES OK, INSTALACION OK, MML OK,
+[2023-03-24 11:13:45] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: ANT7136 ATP TX: Se observa niveles RX  cerca a los calculados por ingeniería OK, Se observa buena  Instalación, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 </v>
       </c>
       <c r="CU19" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/ANT7136/Instalacion_RF/ATP-RF_ANT7136_HUAWEI_02-03-2023.xlsx
-http://190.145.9.251/ftpsti/TowerTrack/ANT7136/Instalacion_TX/ATP-TX_ANT7136_NEC_09-03-2023.zip
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/ANT7136/Instalacion_TX/ATP-TX_ANT7136_NEC_09-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/ANT7136/Instalacion_RF/ATP-RF_ANT7136_HUAWEI_02-03-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7136/OC/RNP_ANT7136_TOWER3_22-07-2022.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7136/Tx/ANT7136_E2E-1_10-11-2022.xlsx
 </v>
@@ -4624,7 +4655,10 @@
         <v>44985</v>
       </c>
       <c r="CP20" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ20" s="1">
+        <v>44987</v>
       </c>
       <c r="CR20" t="str">
         <v>SI</v>
@@ -4713,7 +4747,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X21" s="1">
-        <v>45139</v>
+        <v>45148</v>
       </c>
       <c r="AA21">
         <v>34</v>
@@ -4799,7 +4833,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N22">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O22" t="str">
         <v>5.Instalación RF</v>
@@ -4817,10 +4851,10 @@
         <v>44831</v>
       </c>
       <c r="X22" s="1">
-        <v>45026</v>
+        <v>45031</v>
       </c>
       <c r="Y22" s="1">
-        <v>45026</v>
+        <v>45031</v>
       </c>
       <c r="AA22">
         <v>17</v>
@@ -4829,7 +4863,7 @@
         <v>45035</v>
       </c>
       <c r="AC22" s="1">
-        <v>45018</v>
+        <v>45031</v>
       </c>
       <c r="AF22" s="1">
         <v>44979</v>
@@ -4901,13 +4935,13 @@
         <v>READY. OC E2E 20690661</v>
       </c>
       <c r="BR22" s="1">
-        <v>45044</v>
+        <v>45038</v>
       </c>
       <c r="BW22" s="1">
         <v>45046</v>
       </c>
       <c r="BZ22" s="1">
-        <v>45047</v>
+        <v>45040</v>
       </c>
       <c r="CE22" t="str">
         <v>Pendiente vendor</v>
@@ -6531,10 +6565,10 @@
         <v>44802</v>
       </c>
       <c r="X31" s="1">
-        <v>45042</v>
+        <v>45055</v>
       </c>
       <c r="Y31" s="1">
-        <v>45042</v>
+        <v>45055</v>
       </c>
       <c r="AA31">
         <v>20</v>
@@ -6543,7 +6577,7 @@
         <v>45056</v>
       </c>
       <c r="AC31" s="1">
-        <v>45029</v>
+        <v>45043</v>
       </c>
       <c r="AG31" t="str">
         <v>Pendiente vendor</v>
@@ -7311,7 +7345,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N36">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="O36" t="str">
         <v>1.SAQ</v>
@@ -7362,10 +7396,10 @@
         <v>9999999</v>
       </c>
       <c r="BR36" s="1">
-        <v>45202</v>
+        <v>45231</v>
       </c>
       <c r="BZ36" s="1">
-        <v>45204</v>
+        <v>45234</v>
       </c>
       <c r="CE36" t="str">
         <v>Pendiente vendor</v>
@@ -7427,7 +7461,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N37">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="O37" t="str">
         <v>3.Power</v>
@@ -7445,19 +7479,19 @@
         <v>44795</v>
       </c>
       <c r="X37" s="1">
-        <v>45033</v>
+        <v>45066</v>
       </c>
       <c r="Y37" s="1">
-        <v>45033</v>
+        <v>45066</v>
       </c>
       <c r="AA37">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AB37" s="1">
-        <v>45046</v>
+        <v>45080</v>
       </c>
       <c r="AC37" s="1">
-        <v>45020</v>
+        <v>45061</v>
       </c>
       <c r="AG37" t="str">
         <v>Pendiente vendor</v>
@@ -7493,10 +7527,10 @@
         <v>44979</v>
       </c>
       <c r="BR37" s="1">
-        <v>45051</v>
+        <v>45085</v>
       </c>
       <c r="BZ37" s="1">
-        <v>45054</v>
+        <v>45088</v>
       </c>
       <c r="CE37" t="str">
         <v>Pendiente vendor</v>
@@ -8215,7 +8249,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N43">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="O43" t="str">
         <v>1.SAQ</v>
@@ -8281,10 +8315,10 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR43" s="1">
-        <v>45202</v>
+        <v>45231</v>
       </c>
       <c r="BZ43" s="1">
-        <v>45204</v>
+        <v>45234</v>
       </c>
       <c r="CE43" t="str">
         <v>Pendiente vendor</v>
@@ -8347,7 +8381,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N44">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="O44" t="str">
         <v>1.SAQ</v>
@@ -8410,10 +8444,10 @@
         <v>44775</v>
       </c>
       <c r="BR44" s="1">
-        <v>45202</v>
+        <v>45231</v>
       </c>
       <c r="BZ44" s="1">
-        <v>45204</v>
+        <v>45234</v>
       </c>
       <c r="CE44" t="str">
         <v>Pendiente vendor</v>
@@ -9790,7 +9824,10 @@
         <v>44994</v>
       </c>
       <c r="CH52" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CI52" s="1">
+        <v>45009</v>
       </c>
       <c r="CJ52">
         <v>20713229</v>
@@ -9802,7 +9839,10 @@
         <v>44986</v>
       </c>
       <c r="CP52" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ52" s="1">
+        <v>44987</v>
       </c>
       <c r="CR52" t="str">
         <v>SI</v>
@@ -9820,11 +9860,12 @@
 [2023-03-09 14:25:20] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
 [2023-03-09 15:26:25] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO CON PENDIENTES: SOPORTE APROBADO CON PENDIENTES: CHO7033 ATP TX Satelital : Se evidencia Instalación OK, Pruebas TH 4Mb/2Mb RFC OK, FOTOS OK, SERIES OK, Pendiente evidencias sobre las pruebas de Saturacion.
 [2023-03-10 07:53:21] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7033    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI, Nota: tiene 4 correos de solicitud autorizaciones
+[2023-03-24 11:40:03] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: CHO7033 ATP RF: Pagina COVER OK, Medición VSWR OK, Alarmas Menores, CROSS OK, Configuración de Parametros   MML Command OK, Seriales OK, Sitio en Operación.
 </v>
       </c>
       <c r="CU52" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7033/Instalacion_TX/ATP-TX_CHO7033_AXESS_27-02-2023.pdf
-http://190.145.9.251/ftpsti/TowerTrack/CHO7033/Instalacion_RF/ATP-RF_CHO7033_HUAWEI_09-03-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7033/Instalacion_RF/ATP-RF_CHO7033_HUAWEI_09-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7033/Instalacion_TX/ATP-TX_CHO7033_AXESS_27-02-2023.pdf
 http://190.145.9.251/ftpsti/TowerTrack/CHO7033/OC/RNP_CHO7033_TOWER3_08-02-2023.xlsx
 </v>
       </c>
@@ -9867,13 +9908,13 @@
         <v>TOWER 3</v>
       </c>
       <c r="N53">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O53" t="str">
         <v>4.Instalación Tx</v>
       </c>
       <c r="P53" t="str">
-        <v>F1-TX-En E2E 1</v>
+        <v>F5-TX-E2E 2 OK</v>
       </c>
       <c r="S53" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -9885,10 +9926,13 @@
         <v>44729</v>
       </c>
       <c r="X53" s="1">
-        <v>45010</v>
+        <v>45006</v>
       </c>
       <c r="Y53" s="1">
-        <v>45010</v>
+        <v>45006</v>
+      </c>
+      <c r="Z53" s="1">
+        <v>45006</v>
       </c>
       <c r="AA53">
         <v>10</v>
@@ -9962,11 +10006,17 @@
       <c r="BR53" s="1">
         <v>45008</v>
       </c>
+      <c r="BS53" s="1">
+        <v>45008</v>
+      </c>
+      <c r="BT53" s="1">
+        <v>45008</v>
+      </c>
       <c r="BU53" t="str">
-        <v>Soporte para antena Satelital se instalará el 28-03. Fecha en que debe instalar Axess</v>
+        <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
       <c r="BZ53" s="1">
-        <v>45011</v>
+        <v>45014</v>
       </c>
       <c r="CE53" t="str">
         <v>Pendiente vendor</v>
@@ -9992,6 +10042,7 @@
 [2023-02-24 17:30:52] (Luis Collazos) Comentarios E2E 2: Sitio con prolema de orden público reportado el 24-02. En espera de confirmación
 [2023-03-06 10:23:33] (Luis Collazos) Comentarios E2E 2: En espera confirmación Axess de instalación en torre de acuerdo a propuesta de TowerOne
 [2023-03-10 18:05:41] (Luis Collazos) Comentarios E2E 2: Soporte para antena Satelital se instalará el 28-03. Fecha en que debe instalar Axess
+[2023-03-23 15:57:11] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 </v>
       </c>
       <c r="CU53" t="str" xml:space="preserve">
@@ -11149,6 +11200,9 @@
       <c r="BU58" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
+      <c r="BV58" s="1">
+        <v>45008</v>
+      </c>
       <c r="BW58" s="1">
         <v>44639</v>
       </c>
@@ -11443,7 +11497,10 @@
         <v>44999</v>
       </c>
       <c r="CP59" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ59" s="1">
+        <v>44995</v>
       </c>
       <c r="CR59" t="str">
         <v>SI</v>
@@ -12255,7 +12312,10 @@
         <v>44979</v>
       </c>
       <c r="CP63" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ63" s="1">
+        <v>44995</v>
       </c>
       <c r="CR63" t="str">
         <v>SI</v>
@@ -12324,10 +12384,10 @@
         <v>13</v>
       </c>
       <c r="O64" t="str">
-        <v>6.ON AIR</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P64" t="str">
-        <v>F1-OA-ON AIR</v>
+        <v>F1-RAD-OC en ejecución</v>
       </c>
       <c r="S64" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -12425,9 +12485,24 @@
       <c r="BM64" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
+      <c r="BO64" s="1">
+        <v>44986</v>
+      </c>
+      <c r="BP64" s="1">
+        <v>44999</v>
+      </c>
+      <c r="BQ64" s="1">
+        <v>45004</v>
+      </c>
       <c r="BR64" s="1">
         <v>45007</v>
       </c>
+      <c r="BS64" s="1">
+        <v>45006</v>
+      </c>
+      <c r="BT64" s="1">
+        <v>45006</v>
+      </c>
       <c r="BU64" t="str">
         <v>Se inetraría RF con TX</v>
       </c>
@@ -12455,8 +12530,17 @@
       <c r="CH64" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="CJ64">
+        <v>20730161</v>
+      </c>
+      <c r="CK64" s="1">
+        <v>45012</v>
+      </c>
       <c r="CP64" t="str">
-        <v>Sin Entregar</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ64" s="1">
+        <v>45006</v>
       </c>
       <c r="CR64" t="str">
         <v>SI</v>
@@ -12654,7 +12738,7 @@
         <v>45006</v>
       </c>
       <c r="CH65" t="str">
-        <v>En revision ESCO/STI</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CJ65">
         <v>20722643</v>
@@ -12666,7 +12750,10 @@
         <v>45000</v>
       </c>
       <c r="CP65" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ65" s="1">
+        <v>44995</v>
       </c>
       <c r="CR65" t="str">
         <v>SI</v>
@@ -12687,6 +12774,7 @@
 [2023-03-06 16:10:30] (Luis Collazos) Comentarios Generales: RF finaliza el 11-03. Se integraría RF con TX
 [2023-03-13 09:02:30] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 [2023-03-21 11:44:16] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
+[2023-03-21 16:24:12] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7049    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS NA, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
 </v>
       </c>
       <c r="CU65" t="str" xml:space="preserve">
@@ -12736,10 +12824,10 @@
         <v>13</v>
       </c>
       <c r="O66" t="str">
-        <v>4.Instalación Tx</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P66" t="str">
-        <v>F1-TX-En E2E 1</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S66" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -12834,14 +12922,47 @@
       <c r="BR66" s="1">
         <v>45007</v>
       </c>
+      <c r="BS66" s="1">
+        <v>45006</v>
+      </c>
+      <c r="BT66" s="1">
+        <v>45006</v>
+      </c>
+      <c r="BU66" t="str">
+        <v>Instalación Finalizada Pdte E2e y ATP</v>
+      </c>
+      <c r="BW66" s="1">
+        <v>45003</v>
+      </c>
+      <c r="BX66" s="1">
+        <v>45003</v>
+      </c>
+      <c r="BY66" s="1">
+        <v>45007</v>
+      </c>
       <c r="BZ66" s="1">
         <v>45008</v>
       </c>
+      <c r="CA66" s="1">
+        <v>45008</v>
+      </c>
+      <c r="CB66" s="1">
+        <v>45008</v>
+      </c>
       <c r="CE66" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="CH66" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ66">
+        <v>20729329</v>
+      </c>
+      <c r="CK66" s="1">
+        <v>45010</v>
+      </c>
+      <c r="CL66" s="1">
+        <v>45009</v>
       </c>
       <c r="CP66" t="str">
         <v>Sin Entregar</v>
@@ -12858,6 +12979,7 @@
 [2023-03-05 19:20:29] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE RECHAZADO: Requiere validación con fotografías en sitio, teniendo en cuenta que la Base de datos de terreno presenta diferencias con la base de datos de terreno de TesAmerica donde no la altura del cerro es menor y por lo tanto no generaría obstrucción
 [2023-03-15 12:04:26] (Jaime Meza) Fecha Envio RNP - RNP: SOPORTE CORREGIDO: Se añade torre 48 mts (45 mts efectivos por soportería) Version 2
 [2023-03-15 12:16:32] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION 1 - Estructura de 48mts
+[2023-03-22 16:13:08] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 </v>
       </c>
       <c r="CU66" t="str" xml:space="preserve">
@@ -12903,13 +13025,13 @@
         <v>TOWER 3</v>
       </c>
       <c r="N67">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O67" t="str">
-        <v>3.Power</v>
+        <v>4.Instalación Tx</v>
       </c>
       <c r="P67" t="str">
-        <v>F1-PW-En instalación</v>
+        <v>F5-TX-E2E 2 OK</v>
       </c>
       <c r="S67" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -12933,11 +13055,14 @@
         <v>13</v>
       </c>
       <c r="AB67" s="1">
-        <v>45006</v>
+        <v>45008</v>
       </c>
       <c r="AC67" s="1">
         <v>44997</v>
       </c>
+      <c r="AD67" s="1">
+        <v>45008</v>
+      </c>
       <c r="AF67" s="1">
         <v>44985</v>
       </c>
@@ -13002,10 +13127,19 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR67" s="1">
-        <v>45008</v>
+        <v>45014</v>
+      </c>
+      <c r="BS67" s="1">
+        <v>45013</v>
+      </c>
+      <c r="BT67" s="1">
+        <v>45013</v>
+      </c>
+      <c r="BU67" t="str">
+        <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
       <c r="BZ67" s="1">
-        <v>45011</v>
+        <v>45014</v>
       </c>
       <c r="CE67" t="str">
         <v>Pendiente vendor</v>
@@ -13026,6 +13160,7 @@
         <v xml:space="preserve">[2023-02-28 20:49:46] (Jaime Meza) Archivo Subido (Fecha Envio RNP - RNP): Version 1
 [2023-03-01 09:44:54] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2023-03-05 19:28:34] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION 1
+[2023-03-28 15:55:06] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 </v>
       </c>
       <c r="CU67" t="str" xml:space="preserve">
@@ -16740,7 +16875,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N85">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O85" t="str">
         <v>3.Power</v>
@@ -16770,7 +16905,7 @@
         <v>45053</v>
       </c>
       <c r="AC85" s="1">
-        <v>45008</v>
+        <v>45026</v>
       </c>
       <c r="AF85" s="1">
         <v>44985</v>
@@ -16830,16 +16965,16 @@
         <v>44986</v>
       </c>
       <c r="BL85" s="1">
-        <v>44986</v>
+        <v>45009</v>
       </c>
       <c r="BM85" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR85" s="1">
-        <v>45057</v>
+        <v>45058</v>
       </c>
       <c r="BZ85" s="1">
-        <v>45059</v>
+        <v>45061</v>
       </c>
       <c r="CE85" t="str">
         <v>Pendiente vendor</v>
@@ -17506,7 +17641,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N89">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="O89" t="str">
         <v>3.Power</v>
@@ -17524,19 +17659,19 @@
         <v>44820</v>
       </c>
       <c r="X89" s="1">
-        <v>45033</v>
+        <v>45066</v>
       </c>
       <c r="Y89" s="1">
-        <v>45033</v>
+        <v>45066</v>
       </c>
       <c r="AA89">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AB89" s="1">
-        <v>45046</v>
+        <v>45080</v>
       </c>
       <c r="AC89" s="1">
-        <v>45020</v>
+        <v>45061</v>
       </c>
       <c r="AG89" t="str">
         <v>Pendiente vendor</v>
@@ -17572,10 +17707,10 @@
         <v>44979</v>
       </c>
       <c r="BR89" s="1">
-        <v>45051</v>
+        <v>45085</v>
       </c>
       <c r="BZ89" s="1">
-        <v>45054</v>
+        <v>45088</v>
       </c>
       <c r="CE89" t="str">
         <v>Pendiente vendor</v>
@@ -17640,10 +17775,10 @@
         <v>14</v>
       </c>
       <c r="O90" t="str">
-        <v>4.Instalación Tx</v>
+        <v>6.ON AIR</v>
       </c>
       <c r="P90" t="str">
-        <v>F5-TX-E2E 2 OK</v>
+        <v>F1-OA-ON AIR</v>
       </c>
       <c r="S90" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -17750,11 +17885,29 @@
       <c r="BU90" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
+      <c r="BW90" s="1">
+        <v>45005</v>
+      </c>
+      <c r="BX90" s="1">
+        <v>45005</v>
+      </c>
+      <c r="BY90" s="1">
+        <v>45012</v>
+      </c>
       <c r="BZ90" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CA90" s="1">
         <v>45013</v>
       </c>
+      <c r="CB90" s="1">
+        <v>45013</v>
+      </c>
+      <c r="CD90" s="1">
+        <v>45012</v>
+      </c>
       <c r="CE90" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO/STI</v>
       </c>
       <c r="CH90" t="str">
         <v>Pendiente vendor</v>
@@ -17774,10 +17927,12 @@
 [2023-02-28 18:15:28] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design Opcion 1
 [2023-03-01 09:48:29] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2023-03-16 14:22:59] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
+[2023-03-27 10:02:11] (Juan Lozada) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Archivo Subido (Fecha Entrega ATP Tx - ATP Tx)
 </v>
       </c>
       <c r="CU90" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7079/OC/RNP_CHO7079_TOWER3_28-02-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7079/Instalacion_TX/ATP-TX_CHO7079_AXESS_27-03-2023.pdf
+http://190.145.9.251/ftpsti/TowerTrack/CHO7079/OC/RNP_CHO7079_TOWER3_28-02-2023.xlsx
 </v>
       </c>
     </row>
@@ -18054,10 +18209,10 @@
         <v>14</v>
       </c>
       <c r="O92" t="str">
-        <v>3.Power</v>
+        <v>4.Instalación Tx</v>
       </c>
       <c r="P92" t="str">
-        <v>F1-PW-En instalación</v>
+        <v>F1-TX-En E2E 1</v>
       </c>
       <c r="S92" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -18074,6 +18229,9 @@
       <c r="Y92" s="1">
         <v>45053</v>
       </c>
+      <c r="Z92" s="1">
+        <v>45006</v>
+      </c>
       <c r="AA92">
         <v>13</v>
       </c>
@@ -18083,6 +18241,9 @@
       <c r="AC92" s="1">
         <v>45048</v>
       </c>
+      <c r="AD92" s="1">
+        <v>45011</v>
+      </c>
       <c r="AF92" s="1">
         <v>44985</v>
       </c>
@@ -18153,7 +18314,7 @@
         <v>45012</v>
       </c>
       <c r="BZ92" s="1">
-        <v>45013</v>
+        <v>45014</v>
       </c>
       <c r="CE92" t="str">
         <v>Pendiente vendor</v>
@@ -18553,10 +18714,10 @@
         <v>12</v>
       </c>
       <c r="O95" t="str">
-        <v>6.ON AIR</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P95" t="str">
-        <v>F1-OA-ON AIR</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S95" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -18684,8 +18845,20 @@
       <c r="CH95" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="CJ95">
+        <v>20727384</v>
+      </c>
+      <c r="CK95" s="1">
+        <v>45008</v>
+      </c>
+      <c r="CL95" s="1">
+        <v>45005</v>
+      </c>
       <c r="CP95" t="str">
-        <v>Sin Entregar</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ95" s="1">
+        <v>45002</v>
       </c>
       <c r="CR95" t="str">
         <v>SI</v>
@@ -20206,10 +20379,10 @@
         <v>13</v>
       </c>
       <c r="O103" t="str">
-        <v>4.Instalación Tx</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P103" t="str">
-        <v>F1-TX-En E2E 1</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S103" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -20304,11 +20477,41 @@
       <c r="BM103" t="str">
         <v>READY.</v>
       </c>
+      <c r="BO103" s="1">
+        <v>44986</v>
+      </c>
+      <c r="BP103" s="1">
+        <v>44993</v>
+      </c>
+      <c r="BQ103" s="1">
+        <v>44997</v>
+      </c>
       <c r="BR103" s="1">
         <v>44999</v>
       </c>
+      <c r="BS103" s="1">
+        <v>44999</v>
+      </c>
+      <c r="BT103" s="1">
+        <v>44999</v>
+      </c>
+      <c r="BW103" s="1">
+        <v>45004</v>
+      </c>
+      <c r="BX103" s="1">
+        <v>45004</v>
+      </c>
+      <c r="BY103" s="1">
+        <v>45008</v>
+      </c>
       <c r="BZ103" s="1">
-        <v>45008</v>
+        <v>45009</v>
+      </c>
+      <c r="CA103" s="1">
+        <v>45009</v>
+      </c>
+      <c r="CB103" s="1">
+        <v>45009</v>
       </c>
       <c r="CD103" s="1">
         <v>45001</v>
@@ -20318,6 +20521,15 @@
       </c>
       <c r="CH103" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ103">
+        <v>20729329</v>
+      </c>
+      <c r="CK103" s="1">
+        <v>45010</v>
+      </c>
+      <c r="CL103" s="1">
+        <v>45010</v>
       </c>
       <c r="CP103" t="str">
         <v>Sin Entregar</v>
@@ -20982,7 +21194,7 @@
         <v>45006</v>
       </c>
       <c r="CH107" t="str">
-        <v>En revision ESCO/STI</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CJ107">
         <v>20722643</v>
@@ -20994,7 +21206,10 @@
         <v>44997</v>
       </c>
       <c r="CP107" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ107" s="1">
+        <v>44995</v>
       </c>
       <c r="CR107" t="str">
         <v>SI</v>
@@ -21012,6 +21227,7 @@
 [2023-03-13 10:12:09] (Juan Lozada) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Archivo Subido (Fecha Entrega ATP Tx - ATP Tx)
 [2023-03-14 14:26:16] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7098    ATP TX SAT:  Instalación OK, TH 4Mb/2Mb RFC OK, FOTOS OK, SERIES fotos borrosas, SATUR OK¡
 [2023-03-21 11:45:33] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
+[2023-03-22 09:57:40] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7098    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
 </v>
       </c>
       <c r="CU107" t="str" xml:space="preserve">
@@ -22037,6 +22253,9 @@
       <c r="AP114" t="str">
         <v>CHO7106(sat)-CHO7111:CHO7111-CHO0008</v>
       </c>
+      <c r="AQ114" t="str">
+        <v>CHO7106</v>
+      </c>
       <c r="AR114" t="str">
         <v>CHO0008</v>
       </c>
@@ -22701,7 +22920,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N119">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="O119" t="str">
         <v>3.Power</v>
@@ -22719,19 +22938,19 @@
         <v>44789</v>
       </c>
       <c r="X119" s="1">
-        <v>45026</v>
+        <v>45046</v>
       </c>
       <c r="Y119" s="1">
-        <v>45026</v>
+        <v>45046</v>
       </c>
       <c r="AA119">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="AB119" s="1">
-        <v>45040</v>
+        <v>45101</v>
       </c>
       <c r="AC119" s="1">
-        <v>45013</v>
+        <v>45046</v>
       </c>
       <c r="AF119" s="1">
         <v>44979</v>
@@ -22797,10 +23016,10 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR119" s="1">
-        <v>45045</v>
+        <v>45106</v>
       </c>
       <c r="BZ119" s="1">
-        <v>45047</v>
+        <v>45109</v>
       </c>
       <c r="CE119" t="str">
         <v>Pendiente vendor</v>
@@ -23000,8 +23219,11 @@
       <c r="CE120" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="CG120" s="1">
+        <v>45008</v>
+      </c>
       <c r="CH120" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CJ120">
         <v>20722643</v>
@@ -23013,7 +23235,10 @@
         <v>44999</v>
       </c>
       <c r="CP120" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ120" s="1">
+        <v>44995</v>
       </c>
       <c r="CR120" t="str">
         <v>SI</v>
@@ -23033,10 +23258,13 @@
 [2023-03-06 16:08:55] (Luis Collazos) Comentarios E2E 2: Axess llegará el 10-03, fecha en que está programado entregar RF. Se integra RF con TX
 [2023-03-06 16:08:55] (Luis Collazos) Comentarios Generales: RF llega el 08-3 y entregará el eNode el 10-03
 [2023-03-13 09:01:23] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
+[2023-03-23 18:11:26] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
+[2023-03-24 14:26:23] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7113    ATP RF: COVER OK, VSWR OK, ALARM minor, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
 </v>
       </c>
       <c r="CU120" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7113/OC/RNP_CHO7113_TOWER3_21-02-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7113/Instalacion_RF/ATP-RF_CHO7113_HUAWEI_23-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7113/OC/RNP_CHO7113_TOWER3_21-02-2023.xlsx
 </v>
       </c>
     </row>
@@ -24332,10 +24560,10 @@
         <v>44802</v>
       </c>
       <c r="X130" s="1">
-        <v>45061</v>
+        <v>45031</v>
       </c>
       <c r="Y130" s="1">
-        <v>45061</v>
+        <v>45031</v>
       </c>
       <c r="AA130">
         <v>23</v>
@@ -24344,7 +24572,7 @@
         <v>45075</v>
       </c>
       <c r="AC130" s="1">
-        <v>45048</v>
+        <v>45010</v>
       </c>
       <c r="AG130" t="str">
         <v>Pendiente vendor</v>
@@ -24430,7 +24658,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N131">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="O131" t="str">
         <v>3.Power</v>
@@ -24448,19 +24676,19 @@
         <v>44776</v>
       </c>
       <c r="X131" s="1">
-        <v>45031</v>
+        <v>45076</v>
       </c>
       <c r="Y131" s="1">
-        <v>45031</v>
+        <v>45076</v>
       </c>
       <c r="AA131">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AB131" s="1">
-        <v>45045</v>
+        <v>45090</v>
       </c>
       <c r="AC131" s="1">
-        <v>45018</v>
+        <v>45048</v>
       </c>
       <c r="AF131" s="1">
         <v>44992</v>
@@ -24508,10 +24736,10 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR131" s="1">
-        <v>45050</v>
+        <v>45095</v>
       </c>
       <c r="BZ131" s="1">
-        <v>45052</v>
+        <v>45098</v>
       </c>
       <c r="CE131" t="str">
         <v>Pendiente vendor</v>
@@ -25054,13 +25282,13 @@
         <v>TOWER 3</v>
       </c>
       <c r="N134">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O134" t="str">
-        <v>2.Civil Work</v>
+        <v>1.SAQ</v>
       </c>
       <c r="P134" t="str">
-        <v>F1-CW-En construcción</v>
+        <v>F2-SAQ-Contrato Firmado</v>
       </c>
       <c r="S134" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -25072,16 +25300,13 @@
         <v>44992</v>
       </c>
       <c r="X134" s="1">
-        <v>45107</v>
-      </c>
-      <c r="Y134" s="1">
-        <v>45107</v>
+        <v>45140</v>
       </c>
       <c r="AA134">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="AB134" s="1">
-        <v>45121</v>
+        <v>45154</v>
       </c>
       <c r="AF134" s="1">
         <v>44987</v>
@@ -25141,10 +25366,10 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR134" s="1">
-        <v>45126</v>
+        <v>45159</v>
       </c>
       <c r="BZ134" s="1">
-        <v>45128</v>
+        <v>45162</v>
       </c>
       <c r="CE134" t="str">
         <v>Pendiente vendor</v>
@@ -25891,6 +26116,9 @@
       </c>
       <c r="AV138" s="1">
         <v>44832</v>
+      </c>
+      <c r="AW138" t="str">
+        <v>NA</v>
       </c>
       <c r="BD138">
         <v>9999999</v>
@@ -30200,13 +30428,13 @@
         <v>TOWER 3</v>
       </c>
       <c r="N159">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O159" t="str">
-        <v>2.Civil Work</v>
+        <v>1.SAQ</v>
       </c>
       <c r="P159" t="str">
-        <v>F1-CW-En construcción</v>
+        <v>F2-SAQ-Contrato Firmado</v>
       </c>
       <c r="S159" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -30218,16 +30446,13 @@
         <v>44812</v>
       </c>
       <c r="X159" s="1">
-        <v>45077</v>
-      </c>
-      <c r="Y159" s="1">
-        <v>45077</v>
+        <v>45092</v>
       </c>
       <c r="AA159">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AB159" s="1">
-        <v>45091</v>
+        <v>45106</v>
       </c>
       <c r="AG159" t="str">
         <v>Pendiente vendor</v>
@@ -30287,10 +30512,10 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR159" s="1">
-        <v>45096</v>
+        <v>45111</v>
       </c>
       <c r="BZ159" s="1">
-        <v>45098</v>
+        <v>45114</v>
       </c>
       <c r="CE159" t="str">
         <v>Pendiente vendor</v>
@@ -31332,10 +31557,10 @@
         <v>13</v>
       </c>
       <c r="O165" t="str">
-        <v>4.Instalación Tx</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P165" t="str">
-        <v>F1-TX-En E2E 1</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S165" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -31430,17 +31655,56 @@
       <c r="BM165" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
+      <c r="BO165" s="1">
+        <v>44986</v>
+      </c>
+      <c r="BP165" s="1">
+        <v>44995</v>
+      </c>
+      <c r="BQ165" s="1">
+        <v>45002</v>
+      </c>
       <c r="BR165" s="1">
         <v>45004</v>
       </c>
+      <c r="BS165" s="1">
+        <v>45004</v>
+      </c>
+      <c r="BT165" s="1">
+        <v>45004</v>
+      </c>
+      <c r="BW165" s="1">
+        <v>45003</v>
+      </c>
+      <c r="BX165" s="1">
+        <v>45003</v>
+      </c>
+      <c r="BY165" s="1">
+        <v>45006</v>
+      </c>
       <c r="BZ165" s="1">
-        <v>45006</v>
+        <v>45008</v>
+      </c>
+      <c r="CA165" s="1">
+        <v>45007</v>
+      </c>
+      <c r="CB165" s="1">
+        <v>45008</v>
       </c>
       <c r="CE165" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="CH165" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ165">
+        <v>20729329</v>
+      </c>
+      <c r="CK165" s="1">
+        <v>45010</v>
+      </c>
+      <c r="CL165" s="1">
+        <v>45009</v>
       </c>
       <c r="CP165" t="str">
         <v>Sin Entregar</v>
@@ -31500,7 +31764,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N166">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O166" t="str">
         <v>3.Power</v>
@@ -31518,19 +31782,19 @@
         <v>44812</v>
       </c>
       <c r="X166" s="1">
-        <v>45033</v>
+        <v>45076</v>
       </c>
       <c r="Y166" s="1">
-        <v>45033</v>
+        <v>45076</v>
       </c>
       <c r="AA166">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="AB166" s="1">
-        <v>45046</v>
+        <v>45090</v>
       </c>
       <c r="AC166" s="1">
-        <v>45020</v>
+        <v>45050</v>
       </c>
       <c r="AG166" t="str">
         <v>Pendiente vendor</v>
@@ -31551,10 +31815,10 @@
         <v>CHO7171-CHO7078:CHO7078-CHO7077:CHO7077-CHO7184:CHO7184-CHO7106:CHO7106-CHO7111:CHO7111-CHO0008</v>
       </c>
       <c r="BR166" s="1">
-        <v>45051</v>
+        <v>45095</v>
       </c>
       <c r="BZ166" s="1">
-        <v>45054</v>
+        <v>45098</v>
       </c>
       <c r="CE166" t="str">
         <v>Pendiente vendor</v>
@@ -32955,17 +33219,20 @@
       <c r="CB173" s="1">
         <v>44970</v>
       </c>
+      <c r="CD173" s="1">
+        <v>45008</v>
+      </c>
       <c r="CE173" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado con Pendientes STI)</v>
       </c>
       <c r="CG173" s="1">
         <v>44981</v>
       </c>
       <c r="CH173" t="str">
-        <v>Aprobado con Pendientes</v>
+        <v>Aprobado</v>
       </c>
       <c r="CI173" s="1">
-        <v>44991</v>
+        <v>45009</v>
       </c>
       <c r="CJ173">
         <v>20697685</v>
@@ -32999,10 +33266,14 @@
 [2023-03-06 18:52:17] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO CON PENDIENTES: SOPORTE APROBADO CON PENDIENTES: CHO7181 ATP RF: COVER Incompleto, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: OK, Pendiente: completar Cover con info sectores y antenas
 [2023-03-09 16:23:55] (Kevin Guerrero) Fecha Entrega ATP Rf - ATP RF: SOPORTE CORREGIDO: Anexo ATP para revisión, el Cover esta completo Ok.  
 [2023-03-10 10:25:04] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7181 ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: OK,
+[2023-03-23 01:48:06] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacion correspondiente
+[2023-03-23 09:06:27] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO CON PENDIENTES: CHO7181    ATP TX: NIVELES OK, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES falta activo ODU, Personal OK
+[2023-03-24 12:01:39] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: CHO7181 ATP RF: COVER ok, Medición VSWR OK, Sin alarmas, CROSS OK, Configuración de Parámetros  OK, SERIAL OK, INSTALACION OK.
 </v>
       </c>
       <c r="CU173" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7181/Instalacion_RF/ATP-RF_CHO7181_HUAWEI_24-02-2023_VersionFinal.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7181/Instalacion_TX/ATP-TX_CHO7181_NEC_23-03-2023.zip
+http://190.145.9.251/ftpsti/TowerTrack/CHO7181/Instalacion_RF/ATP-RF_CHO7181_HUAWEI_24-02-2023_VersionFinal.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/CHO7181/Instalacion_RF/ATP-RF_CHO7181_HUAWEI_24-02-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/CHO7181/OC/RNP_CHO7181_TOWER 3_30-08-2022.xlsx
 </v>
@@ -33390,7 +33661,7 @@
         <v>Huawei</v>
       </c>
       <c r="L176" t="str">
-        <v>Axess</v>
+        <v>NEC</v>
       </c>
       <c r="M176" t="str">
         <v>TOWER 3</v>
@@ -33447,34 +33718,37 @@
         <v>Pendiente vendor</v>
       </c>
       <c r="AJ176">
-        <v>20522160</v>
+        <v>20643024</v>
       </c>
       <c r="AK176" s="1">
-        <v>44788</v>
+        <v>45012</v>
       </c>
       <c r="AL176" t="str">
         <v>Temporal</v>
       </c>
       <c r="AM176" t="str">
-        <v>Satelital</v>
+        <v>MW + Satelital</v>
       </c>
       <c r="AN176" t="str">
-        <v>Solo MW y/o IRU</v>
+        <v>MW + Satelital</v>
       </c>
       <c r="AO176">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AP176" t="str">
-        <v>CHO7184-SATELITAL</v>
+        <v>CHO7184-CHO7106</v>
+      </c>
+      <c r="AQ176" t="str">
+        <v>CHO7106</v>
       </c>
       <c r="AT176" t="str">
         <v>Axesat</v>
       </c>
       <c r="AU176">
-        <v>63435</v>
+        <v>64245</v>
       </c>
       <c r="AV176" s="1">
-        <v>44784</v>
+        <v>44902</v>
       </c>
       <c r="BD176">
         <v>9999999</v>
@@ -34116,7 +34390,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N179">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O179" t="str">
         <v>4.Instalación Tx</v>
@@ -34215,7 +34489,7 @@
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
       <c r="BZ179" s="1">
-        <v>45009</v>
+        <v>45014</v>
       </c>
       <c r="CE179" t="str">
         <v>Pendiente vendor</v>
@@ -35068,7 +35342,10 @@
         <v>44981</v>
       </c>
       <c r="CP186" t="str">
-        <v>En Revisión</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ186" s="1">
+        <v>44987</v>
       </c>
       <c r="CR186" t="str">
         <v>SI</v>
@@ -35650,7 +35927,7 @@
         <v>44992</v>
       </c>
       <c r="X192" s="1">
-        <v>45177</v>
+        <v>45240</v>
       </c>
       <c r="AA192">
         <v>46</v>
@@ -35840,7 +36117,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N194">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O194" t="str">
         <v>1.SAQ</v>
@@ -35879,10 +36156,10 @@
         <v>CHO7202-CHO7074:CHO7074-CHO7091:CHO7091-CHO7096:CHO7096-CHO7183:CHO7183-CHO7088:CHO7088-CHO0015</v>
       </c>
       <c r="BR194" s="1">
-        <v>45121</v>
+        <v>45146</v>
       </c>
       <c r="BZ194" s="1">
-        <v>45123</v>
+        <v>45149</v>
       </c>
       <c r="CE194" t="str">
         <v>Pendiente vendor</v>
@@ -36048,10 +36325,10 @@
         <v>12</v>
       </c>
       <c r="O196" t="str">
-        <v>6.ON AIR</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P196" t="str">
-        <v>F1-OA-ON AIR</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S196" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -36149,9 +36426,24 @@
       <c r="BM196" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
+      <c r="BO196" s="1">
+        <v>44993</v>
+      </c>
+      <c r="BP196" s="1">
+        <v>44998</v>
+      </c>
+      <c r="BQ196" s="1">
+        <v>45001</v>
+      </c>
       <c r="BR196" s="1">
         <v>45002</v>
       </c>
+      <c r="BS196" s="1">
+        <v>45002</v>
+      </c>
+      <c r="BT196" s="1">
+        <v>45002</v>
+      </c>
       <c r="BU196" t="str">
         <v>Se integraría RF con TX</v>
       </c>
@@ -36173,14 +36465,32 @@
       <c r="CB196" s="1">
         <v>45002</v>
       </c>
+      <c r="CD196" s="1">
+        <v>45013</v>
+      </c>
       <c r="CE196" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO/STI</v>
+      </c>
+      <c r="CG196" s="1">
+        <v>45009</v>
       </c>
       <c r="CH196" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
+      </c>
+      <c r="CJ196">
+        <v>20727384</v>
+      </c>
+      <c r="CK196" s="1">
+        <v>45008</v>
+      </c>
+      <c r="CL196" s="1">
+        <v>45004</v>
       </c>
       <c r="CP196" t="str">
-        <v>Sin Entregar</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ196" s="1">
+        <v>45006</v>
       </c>
       <c r="CR196" t="str">
         <v>SI</v>
@@ -36196,10 +36506,15 @@
 [2023-03-08 16:54:10] (Luis Collazos) Comentarios E2E 2: La punta B cambió
 [2023-03-08 16:58:37] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION  1
 [2023-03-13 08:32:37] (Luis Collazos) Comentarios E2E 2: Se integraría RF con TX
+[2023-03-24 17:44:53] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión.  
+[2023-03-27 15:51:57] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7204    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS NA, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
+[2023-03-28 16:32:59] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacion paa revisión
 </v>
       </c>
       <c r="CU196" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7204/OC/RNP_CHO7204_TOWER3_28-02-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7204/Instalacion_TX/ATP-TX_CHO7204_NEC_28-03-2023.zip
+http://190.145.9.251/ftpsti/TowerTrack/CHO7204/Instalacion_RF/ATP-RF_CHO7204_HUAWEI_24-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7204/OC/RNP_CHO7204_TOWER3_28-02-2023.xlsx
 </v>
       </c>
     </row>
@@ -36241,7 +36556,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N197">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="O197" t="str">
         <v>1.SAQ</v>
@@ -36259,13 +36574,13 @@
         <v>44992</v>
       </c>
       <c r="X197" s="1">
-        <v>45069</v>
+        <v>45127</v>
       </c>
       <c r="AA197">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="AB197" s="1">
-        <v>45083</v>
+        <v>45141</v>
       </c>
       <c r="AL197" t="str">
         <v>Definitiva</v>
@@ -36280,10 +36595,10 @@
         <v>CHO7205-CHO7128:CHO7128-CHO7132:CHO7132-CHO7143:CHO7143-CHO7144:CHO7144-CHO7146:CHO7146-CHO7147:CHO7147-VAC0090</v>
       </c>
       <c r="BR197" s="1">
-        <v>45088</v>
+        <v>45146</v>
       </c>
       <c r="BZ197" s="1">
-        <v>45090</v>
+        <v>45149</v>
       </c>
       <c r="CE197" t="str">
         <v>Pendiente vendor</v>
@@ -36363,7 +36678,7 @@
         <v>44993</v>
       </c>
       <c r="X198" s="1">
-        <v>45177</v>
+        <v>45240</v>
       </c>
       <c r="AA198">
         <v>46</v>
@@ -36467,10 +36782,10 @@
         <v>46022</v>
       </c>
       <c r="AA199">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="AB199" s="1">
-        <v>45305</v>
+        <v>46022</v>
       </c>
       <c r="AL199" t="str">
         <v>Definitiva</v>
@@ -36775,7 +37090,7 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>CHO7213</v>
+        <v>CHO7211</v>
       </c>
       <c r="B203">
         <v>5</v>
@@ -36828,6 +37143,12 @@
       <c r="Y203" s="1">
         <v>45474</v>
       </c>
+      <c r="AA203">
+        <v>30</v>
+      </c>
+      <c r="AB203" s="1">
+        <v>45495</v>
+      </c>
       <c r="CE203" t="str">
         <v>Pendiente vendor</v>
       </c>
@@ -36847,12 +37168,12 @@
         <v/>
       </c>
     </row>
-    <row r="204" xml:space="preserve">
+    <row r="204">
       <c r="A204" t="str">
-        <v>NEW7003</v>
+        <v>CHO7213</v>
       </c>
       <c r="B204">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C204" t="str">
         <v>TOWER 3</v>
@@ -36870,10 +37191,10 @@
         <v>6</v>
       </c>
       <c r="I204" t="str">
-        <v>Res. 333</v>
+        <v>Res. 332</v>
       </c>
       <c r="J204" s="1">
-        <v>44651</v>
+        <v>45781</v>
       </c>
       <c r="K204" t="str">
         <v>Huawei</v>
@@ -36884,14 +37205,11 @@
       <c r="M204" t="str">
         <v>TOWER 3</v>
       </c>
-      <c r="N204">
-        <v>23</v>
-      </c>
       <c r="O204" t="str">
-        <v>1.SAQ</v>
+        <v>2.Civil Work</v>
       </c>
       <c r="P204" t="str">
-        <v>F1-SAQ-Busqueda y Negociación</v>
+        <v>F1-CW-En construcción</v>
       </c>
       <c r="S204" t="str">
         <v>1.HLD</v>
@@ -36900,37 +37218,16 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X204" s="1">
-        <v>45781</v>
+        <v>45474</v>
+      </c>
+      <c r="Y204" s="1">
+        <v>45474</v>
       </c>
       <c r="AA204">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="AB204" s="1">
-        <v>45802</v>
-      </c>
-      <c r="BD204">
-        <v>9999999</v>
-      </c>
-      <c r="BF204">
-        <v>9999999</v>
-      </c>
-      <c r="BH204">
-        <v>9999999</v>
-      </c>
-      <c r="BJ204" s="1">
-        <v>44972</v>
-      </c>
-      <c r="BL204" s="1">
-        <v>44972</v>
-      </c>
-      <c r="BM204" t="str">
-        <v>NA</v>
-      </c>
-      <c r="BR204" s="1">
-        <v>45807</v>
-      </c>
-      <c r="BZ204" s="1">
-        <v>45810</v>
+        <v>45495</v>
       </c>
       <c r="CE204" t="str">
         <v>Pendiente vendor</v>
@@ -36944,9 +37241,8 @@
       <c r="CR204" t="str">
         <v>SI</v>
       </c>
-      <c r="CT204" t="str" xml:space="preserve">
-        <v xml:space="preserve">[2023-02-15 09:24:21] (Sandra Galan) Comentarios E2E 1: NA
-</v>
+      <c r="CT204" t="str">
+        <v/>
       </c>
       <c r="CU204" t="str">
         <v/>
@@ -36954,10 +37250,10 @@
     </row>
     <row r="205" xml:space="preserve">
       <c r="A205" t="str">
-        <v>NEW7015</v>
+        <v>NEW7003</v>
       </c>
       <c r="B205">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C205" t="str">
         <v>TOWER 3</v>
@@ -36978,7 +37274,7 @@
         <v>Res. 333</v>
       </c>
       <c r="J205" s="1">
-        <v>44911</v>
+        <v>44651</v>
       </c>
       <c r="K205" t="str">
         <v>Huawei</v>
@@ -36990,7 +37286,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N205">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="O205" t="str">
         <v>1.SAQ</v>
@@ -37005,13 +37301,13 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X205" s="1">
-        <v>45747</v>
+        <v>45781</v>
       </c>
       <c r="AA205">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AB205" s="1">
-        <v>45761</v>
+        <v>45802</v>
       </c>
       <c r="BD205">
         <v>9999999</v>
@@ -37023,16 +37319,19 @@
         <v>9999999</v>
       </c>
       <c r="BJ205" s="1">
-        <v>44964</v>
+        <v>44972</v>
+      </c>
+      <c r="BL205" s="1">
+        <v>44972</v>
       </c>
       <c r="BM205" t="str">
         <v>NA</v>
       </c>
       <c r="BR205" s="1">
-        <v>45766</v>
+        <v>45807</v>
       </c>
       <c r="BZ205" s="1">
-        <v>45769</v>
+        <v>45810</v>
       </c>
       <c r="CE205" t="str">
         <v>Pendiente vendor</v>
@@ -37046,101 +37345,114 @@
       <c r="CR205" t="str">
         <v>SI</v>
       </c>
-      <c r="CS205" t="str">
+      <c r="CT205" t="str" xml:space="preserve">
+        <v xml:space="preserve">[2023-02-15 09:24:21] (Sandra Galan) Comentarios E2E 1: NA
+</v>
+      </c>
+      <c r="CU205" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="206" xml:space="preserve">
+      <c r="A206" t="str">
+        <v>NEW7015</v>
+      </c>
+      <c r="B206">
+        <v>2</v>
+      </c>
+      <c r="C206" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D206" t="str">
+        <v>DEFINITIVO</v>
+      </c>
+      <c r="F206" t="str">
+        <v>OCCIDENTE</v>
+      </c>
+      <c r="G206" t="str">
+        <v>Andina</v>
+      </c>
+      <c r="H206">
+        <v>6</v>
+      </c>
+      <c r="I206" t="str">
+        <v>Res. 333</v>
+      </c>
+      <c r="J206" s="1">
+        <v>44911</v>
+      </c>
+      <c r="K206" t="str">
+        <v>Huawei</v>
+      </c>
+      <c r="L206" t="str">
+        <v>Por definir</v>
+      </c>
+      <c r="M206" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N206">
+        <v>17</v>
+      </c>
+      <c r="O206" t="str">
+        <v>1.SAQ</v>
+      </c>
+      <c r="P206" t="str">
+        <v>F1-SAQ-Busqueda y Negociación</v>
+      </c>
+      <c r="S206" t="str">
+        <v>1.HLD</v>
+      </c>
+      <c r="T206" t="str">
+        <v>F0-HLD-No iniciado</v>
+      </c>
+      <c r="X206" s="1">
+        <v>45747</v>
+      </c>
+      <c r="AA206">
+        <v>16</v>
+      </c>
+      <c r="AB206" s="1">
+        <v>45761</v>
+      </c>
+      <c r="BD206">
+        <v>9999999</v>
+      </c>
+      <c r="BF206">
+        <v>9999999</v>
+      </c>
+      <c r="BH206">
+        <v>9999999</v>
+      </c>
+      <c r="BJ206" s="1">
+        <v>44964</v>
+      </c>
+      <c r="BM206" t="str">
+        <v>NA</v>
+      </c>
+      <c r="BR206" s="1">
+        <v>45766</v>
+      </c>
+      <c r="BZ206" s="1">
+        <v>45769</v>
+      </c>
+      <c r="CE206" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="CH206" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="CP206" t="str">
+        <v>Sin Entregar</v>
+      </c>
+      <c r="CR206" t="str">
+        <v>SI</v>
+      </c>
+      <c r="CS206" t="str">
         <v>3 Adicional</v>
       </c>
-      <c r="CT205" t="str" xml:space="preserve">
+      <c r="CT206" t="str" xml:space="preserve">
         <v xml:space="preserve">[2023-02-07 08:27:02] (Sandra Galan) Comentarios E2E 1: NA
 </v>
-      </c>
-      <c r="CU205" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="str">
-        <v>NEW7017</v>
-      </c>
-      <c r="B206">
-        <v>5</v>
-      </c>
-      <c r="C206" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D206" t="str">
-        <v>DEFINITIVO</v>
-      </c>
-      <c r="F206" t="str">
-        <v>OCCIDENTE</v>
-      </c>
-      <c r="G206" t="str">
-        <v>Andina</v>
-      </c>
-      <c r="H206">
-        <v>6</v>
-      </c>
-      <c r="I206" t="str">
-        <v>Res. 332</v>
-      </c>
-      <c r="J206" s="1">
-        <v>45781</v>
-      </c>
-      <c r="K206" t="str">
-        <v>Huawei</v>
-      </c>
-      <c r="L206" t="str">
-        <v>Por definir</v>
-      </c>
-      <c r="M206" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N206">
-        <v>47</v>
-      </c>
-      <c r="O206" t="str">
-        <v>1.SAQ</v>
-      </c>
-      <c r="P206" t="str">
-        <v>F1-SAQ-Busqueda y Negociación</v>
-      </c>
-      <c r="S206" t="str">
-        <v>1.HLD</v>
-      </c>
-      <c r="T206" t="str">
-        <v>F0-HLD-No iniciado</v>
-      </c>
-      <c r="X206" s="1">
-        <v>45585</v>
-      </c>
-      <c r="AA206">
-        <v>45</v>
-      </c>
-      <c r="AB206" s="1">
-        <v>45605</v>
-      </c>
-      <c r="BR206" s="1">
-        <v>45612</v>
-      </c>
-      <c r="BZ206" s="1">
-        <v>45615</v>
-      </c>
-      <c r="CE206" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="CH206" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="CP206" t="str">
-        <v>Sin Entregar</v>
-      </c>
-      <c r="CR206" t="str">
-        <v>SI</v>
-      </c>
-      <c r="CS206" t="str">
-        <v>5</v>
-      </c>
-      <c r="CT206" t="str">
-        <v/>
       </c>
       <c r="CU206" t="str">
         <v/>
@@ -37148,7 +37460,7 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>NEW7018</v>
+        <v>NEW7017</v>
       </c>
       <c r="B207">
         <v>5</v>
@@ -37184,7 +37496,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N207">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="O207" t="str">
         <v>1.SAQ</v>
@@ -37199,19 +37511,19 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X207" s="1">
-        <v>45781</v>
+        <v>45585</v>
       </c>
       <c r="AA207">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="AB207" s="1">
-        <v>45795</v>
+        <v>45605</v>
       </c>
       <c r="BR207" s="1">
-        <v>45802</v>
+        <v>45612</v>
       </c>
       <c r="BZ207" s="1">
-        <v>45807</v>
+        <v>45615</v>
       </c>
       <c r="CE207" t="str">
         <v>Pendiente vendor</v>
@@ -37235,12 +37547,12 @@
         <v/>
       </c>
     </row>
-    <row r="208" xml:space="preserve">
+    <row r="208">
       <c r="A208" t="str">
-        <v>RIS7001</v>
+        <v>NEW7018</v>
       </c>
       <c r="B208">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C208" t="str">
         <v>TOWER 3</v>
@@ -37261,189 +37573,278 @@
         <v>Res. 332</v>
       </c>
       <c r="J208" s="1">
-        <v>45050</v>
+        <v>45781</v>
       </c>
       <c r="K208" t="str">
         <v>Huawei</v>
       </c>
       <c r="L208" t="str">
-        <v>Axess</v>
+        <v>Por definir</v>
       </c>
       <c r="M208" t="str">
         <v>TOWER 3</v>
       </c>
       <c r="N208">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="O208" t="str">
-        <v>7.Integración RAD II</v>
+        <v>1.SAQ</v>
       </c>
       <c r="P208" t="str">
-        <v>F2-RAD-Integrado RAD II</v>
+        <v>F1-SAQ-Busqueda y Negociación</v>
       </c>
       <c r="S208" t="str">
-        <v>2.Configuración TX (E2E 1-MSP)</v>
+        <v>1.HLD</v>
       </c>
       <c r="T208" t="str">
-        <v>F4-TX-E2E 1 OK</v>
-      </c>
-      <c r="W208" s="1">
-        <v>44729</v>
+        <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X208" s="1">
-        <v>44822</v>
-      </c>
-      <c r="Y208" s="1">
-        <v>44822</v>
-      </c>
-      <c r="Z208" s="1">
-        <v>44822</v>
+        <v>45781</v>
       </c>
       <c r="AA208">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AB208" s="1">
-        <v>44955</v>
-      </c>
-      <c r="AC208" s="1">
-        <v>44819</v>
-      </c>
-      <c r="AD208" s="1">
-        <v>44950</v>
-      </c>
-      <c r="AF208" s="1">
-        <v>44852</v>
-      </c>
-      <c r="AG208" t="str">
-        <v>RNP OK</v>
-      </c>
-      <c r="AI208" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AJ208">
-        <v>20533723</v>
-      </c>
-      <c r="AK208" s="1">
-        <v>44801</v>
-      </c>
-      <c r="AL208" t="str">
-        <v>Temporal</v>
-      </c>
-      <c r="AM208" t="str">
-        <v>Satelital</v>
-      </c>
-      <c r="AN208" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="AO208">
-        <v>0</v>
-      </c>
-      <c r="AP208" t="str">
-        <v>RIS7001-SATELITAL</v>
-      </c>
-      <c r="AT208" t="str">
-        <v>NA</v>
-      </c>
-      <c r="AU208">
-        <v>63502</v>
-      </c>
-      <c r="AV208" s="1">
-        <v>44798</v>
-      </c>
-      <c r="BD208">
-        <v>9999999</v>
-      </c>
-      <c r="BF208">
-        <v>20342350</v>
-      </c>
-      <c r="BG208" s="1">
-        <v>44270</v>
-      </c>
-      <c r="BH208">
-        <v>9999999</v>
-      </c>
-      <c r="BJ208" s="1">
-        <v>44838</v>
-      </c>
-      <c r="BL208" s="1">
-        <v>44838</v>
-      </c>
-      <c r="BM208" t="str">
-        <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
-      </c>
-      <c r="BO208" s="1">
-        <v>44936</v>
+        <v>45795</v>
       </c>
       <c r="BR208" s="1">
-        <v>44962</v>
-      </c>
-      <c r="BS208" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BT208" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BU208" t="str">
-        <v>Instalación Finalizada Pdte E2e y ATP</v>
-      </c>
-      <c r="BW208" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BX208" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BY208" s="1">
-        <v>44965</v>
+        <v>45802</v>
       </c>
       <c r="BZ208" s="1">
-        <v>44967</v>
-      </c>
-      <c r="CA208" s="1">
-        <v>44967</v>
-      </c>
-      <c r="CB208" s="1">
-        <v>44967</v>
-      </c>
-      <c r="CD208" s="1">
-        <v>44971</v>
+        <v>45807</v>
       </c>
       <c r="CE208" t="str">
-        <v>Aprobado</v>
-      </c>
-      <c r="CF208" s="1">
-        <v>44974</v>
-      </c>
-      <c r="CG208" s="1">
-        <v>44977</v>
+        <v>Pendiente vendor</v>
       </c>
       <c r="CH208" t="str">
-        <v>Aprobado con Pendientes</v>
-      </c>
-      <c r="CI208" s="1">
-        <v>44991</v>
-      </c>
-      <c r="CJ208">
-        <v>20697685</v>
-      </c>
-      <c r="CK208" s="1">
-        <v>44971</v>
-      </c>
-      <c r="CL208" s="1">
-        <v>44971</v>
+        <v>Pendiente vendor</v>
       </c>
       <c r="CP208" t="str">
-        <v>Aprobada</v>
-      </c>
-      <c r="CQ208" s="1">
-        <v>44970</v>
+        <v>Sin Entregar</v>
       </c>
       <c r="CR208" t="str">
         <v>SI</v>
       </c>
       <c r="CS208" t="str">
+        <v>5</v>
+      </c>
+      <c r="CT208" t="str">
+        <v/>
+      </c>
+      <c r="CU208" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="209" xml:space="preserve">
+      <c r="A209" t="str">
+        <v>RIS7001</v>
+      </c>
+      <c r="B209">
         <v>3</v>
       </c>
-      <c r="CT208" t="str" xml:space="preserve">
+      <c r="C209" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D209" t="str">
+        <v>DEFINITIVO</v>
+      </c>
+      <c r="F209" t="str">
+        <v>OCCIDENTE</v>
+      </c>
+      <c r="G209" t="str">
+        <v>Andina</v>
+      </c>
+      <c r="H209">
+        <v>6</v>
+      </c>
+      <c r="I209" t="str">
+        <v>Res. 332</v>
+      </c>
+      <c r="J209" s="1">
+        <v>45050</v>
+      </c>
+      <c r="K209" t="str">
+        <v>Huawei</v>
+      </c>
+      <c r="L209" t="str">
+        <v>Axess</v>
+      </c>
+      <c r="M209" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N209">
+        <v>7</v>
+      </c>
+      <c r="O209" t="str">
+        <v>7.Integración RAD II</v>
+      </c>
+      <c r="P209" t="str">
+        <v>F2-RAD-Integrado RAD II</v>
+      </c>
+      <c r="S209" t="str">
+        <v>2.Configuración TX (E2E 1-MSP)</v>
+      </c>
+      <c r="T209" t="str">
+        <v>F4-TX-E2E 1 OK</v>
+      </c>
+      <c r="W209" s="1">
+        <v>44729</v>
+      </c>
+      <c r="X209" s="1">
+        <v>44822</v>
+      </c>
+      <c r="Y209" s="1">
+        <v>44822</v>
+      </c>
+      <c r="Z209" s="1">
+        <v>44822</v>
+      </c>
+      <c r="AA209">
+        <v>5</v>
+      </c>
+      <c r="AB209" s="1">
+        <v>44955</v>
+      </c>
+      <c r="AC209" s="1">
+        <v>44819</v>
+      </c>
+      <c r="AD209" s="1">
+        <v>44950</v>
+      </c>
+      <c r="AF209" s="1">
+        <v>44852</v>
+      </c>
+      <c r="AG209" t="str">
+        <v>RNP OK</v>
+      </c>
+      <c r="AI209" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ209">
+        <v>20533723</v>
+      </c>
+      <c r="AK209" s="1">
+        <v>44801</v>
+      </c>
+      <c r="AL209" t="str">
+        <v>Temporal</v>
+      </c>
+      <c r="AM209" t="str">
+        <v>Satelital</v>
+      </c>
+      <c r="AN209" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AO209">
+        <v>0</v>
+      </c>
+      <c r="AP209" t="str">
+        <v>RIS7001-SATELITAL</v>
+      </c>
+      <c r="AT209" t="str">
+        <v>NA</v>
+      </c>
+      <c r="AU209">
+        <v>63502</v>
+      </c>
+      <c r="AV209" s="1">
+        <v>44798</v>
+      </c>
+      <c r="BD209">
+        <v>9999999</v>
+      </c>
+      <c r="BF209">
+        <v>20342350</v>
+      </c>
+      <c r="BG209" s="1">
+        <v>44270</v>
+      </c>
+      <c r="BH209">
+        <v>9999999</v>
+      </c>
+      <c r="BJ209" s="1">
+        <v>44838</v>
+      </c>
+      <c r="BL209" s="1">
+        <v>44838</v>
+      </c>
+      <c r="BM209" t="str">
+        <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
+      </c>
+      <c r="BO209" s="1">
+        <v>44936</v>
+      </c>
+      <c r="BR209" s="1">
+        <v>44962</v>
+      </c>
+      <c r="BS209" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BT209" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BU209" t="str">
+        <v>Instalación Finalizada Pdte E2e y ATP</v>
+      </c>
+      <c r="BW209" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BX209" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BY209" s="1">
+        <v>44965</v>
+      </c>
+      <c r="BZ209" s="1">
+        <v>44967</v>
+      </c>
+      <c r="CA209" s="1">
+        <v>44967</v>
+      </c>
+      <c r="CB209" s="1">
+        <v>44967</v>
+      </c>
+      <c r="CD209" s="1">
+        <v>44971</v>
+      </c>
+      <c r="CE209" t="str">
+        <v>Aprobado</v>
+      </c>
+      <c r="CF209" s="1">
+        <v>44974</v>
+      </c>
+      <c r="CG209" s="1">
+        <v>44977</v>
+      </c>
+      <c r="CH209" t="str">
+        <v>Aprobado con Pendientes</v>
+      </c>
+      <c r="CI209" s="1">
+        <v>44991</v>
+      </c>
+      <c r="CJ209">
+        <v>20697685</v>
+      </c>
+      <c r="CK209" s="1">
+        <v>44971</v>
+      </c>
+      <c r="CL209" s="1">
+        <v>44971</v>
+      </c>
+      <c r="CP209" t="str">
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ209" s="1">
+        <v>44970</v>
+      </c>
+      <c r="CR209" t="str">
+        <v>SI</v>
+      </c>
+      <c r="CS209" t="str">
+        <v>3</v>
+      </c>
+      <c r="CT209" t="str" xml:space="preserve">
         <v xml:space="preserve">[2022-07-26 16:46:11] (Mayra Martinez) Archivo Subido (Fecha Envio RNP - RNP): RNP RIS7001
 [2022-10-04 13:35:27] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2022-10-14 06:32:19] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE RECHAZADO: Validar ajuste de azimuth y Tilt ya que no da cobertura sobre el mayor centro poblado
@@ -37460,222 +37861,222 @@
 [2023-03-06 17:26:05] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO CON PENDIENTES:  SOPORTE APROBADO CON PENDIENTES: Pestaña COVER OK, Medicion VSWR OK, Sin ALARM presentes, PARAM obtenidos mediante MML OK, SERIAL: antena 1 y 2 sin serial tigo, INSTALACION OK, Se observa muy poco trafico.
 </v>
       </c>
-      <c r="CU208" t="str" xml:space="preserve">
+      <c r="CU209" t="str" xml:space="preserve">
         <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/RIS7001/Instalacion_RF/ATP-RF_RIS7001_HUAWEI_20-02-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7001/Instalacion_TX/ATP-TX_RIS7001_AXESS_14-02-2023.pdf
 http://190.145.9.251/ftpsti/TowerTrack/RIS7001/OC/RNP_RIS7001_TOWER3_26-07-2022.xlsx
 </v>
       </c>
     </row>
-    <row r="209" xml:space="preserve">
-      <c r="A209" t="str">
+    <row r="210" xml:space="preserve">
+      <c r="A210" t="str">
         <v>RIS7002</v>
       </c>
-      <c r="B209">
+      <c r="B210">
         <v>3</v>
       </c>
-      <c r="C209" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D209" t="str">
+      <c r="C210" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D210" t="str">
         <v>DEFINITIVO</v>
       </c>
-      <c r="F209" t="str">
+      <c r="F210" t="str">
         <v>OCCIDENTE</v>
       </c>
-      <c r="G209" t="str">
+      <c r="G210" t="str">
         <v>Andina</v>
       </c>
-      <c r="H209">
+      <c r="H210">
         <v>6</v>
       </c>
-      <c r="I209" t="str">
+      <c r="I210" t="str">
         <v>Res. 332</v>
       </c>
-      <c r="J209" s="1">
+      <c r="J210" s="1">
         <v>45050</v>
       </c>
-      <c r="K209" t="str">
+      <c r="K210" t="str">
         <v>Huawei</v>
       </c>
-      <c r="L209" t="str">
+      <c r="L210" t="str">
         <v>Axess</v>
       </c>
-      <c r="M209" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N209">
+      <c r="M210" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N210">
         <v>8</v>
       </c>
-      <c r="O209" t="str">
+      <c r="O210" t="str">
         <v>7.Integración RAD II</v>
       </c>
-      <c r="P209" t="str">
+      <c r="P210" t="str">
         <v>F2-RAD-Integrado RAD II</v>
       </c>
-      <c r="S209" t="str">
+      <c r="S210" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
-      <c r="T209" t="str">
+      <c r="T210" t="str">
         <v>F4-TX-E2E 1 OK</v>
       </c>
-      <c r="W209" s="1">
+      <c r="W210" s="1">
         <v>44659</v>
       </c>
-      <c r="X209" s="1">
+      <c r="X210" s="1">
         <v>44802</v>
       </c>
-      <c r="Y209" s="1">
+      <c r="Y210" s="1">
         <v>44802</v>
       </c>
-      <c r="Z209" s="1">
+      <c r="Z210" s="1">
         <v>44802</v>
       </c>
-      <c r="AA209">
+      <c r="AA210">
         <v>6</v>
       </c>
-      <c r="AB209" s="1">
+      <c r="AB210" s="1">
         <v>44962</v>
       </c>
-      <c r="AC209" s="1">
+      <c r="AC210" s="1">
         <v>44799</v>
       </c>
-      <c r="AD209" s="1">
+      <c r="AD210" s="1">
         <v>44961</v>
       </c>
-      <c r="AF209" s="1">
+      <c r="AF210" s="1">
         <v>44852</v>
       </c>
-      <c r="AG209" t="str">
+      <c r="AG210" t="str">
         <v>RNP OK</v>
       </c>
-      <c r="AI209" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AJ209">
+      <c r="AI210" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ210">
         <v>20509315</v>
       </c>
-      <c r="AK209" s="1">
+      <c r="AK210" s="1">
         <v>44777</v>
       </c>
-      <c r="AL209" t="str">
+      <c r="AL210" t="str">
         <v>Definitiva</v>
       </c>
-      <c r="AM209" t="str">
+      <c r="AM210" t="str">
         <v>Satelital</v>
       </c>
-      <c r="AN209" t="str">
+      <c r="AN210" t="str">
         <v>N/A</v>
       </c>
-      <c r="AO209">
+      <c r="AO210">
         <v>0</v>
       </c>
-      <c r="AP209" t="str">
+      <c r="AP210" t="str">
         <v>RIS7002-SATELITAL</v>
       </c>
-      <c r="AT209" t="str">
+      <c r="AT210" t="str">
         <v>Axesat</v>
       </c>
-      <c r="AU209">
+      <c r="AU210">
         <v>63349</v>
       </c>
-      <c r="AV209" s="1">
+      <c r="AV210" s="1">
         <v>44775</v>
       </c>
-      <c r="BD209">
+      <c r="BD210">
         <v>9999999</v>
       </c>
-      <c r="BF209">
+      <c r="BF210">
         <v>20244935</v>
       </c>
-      <c r="BG209" s="1">
+      <c r="BG210" s="1">
         <v>44543</v>
       </c>
-      <c r="BH209">
+      <c r="BH210">
         <v>9999999</v>
       </c>
-      <c r="BJ209" s="1">
+      <c r="BJ210" s="1">
         <v>44838</v>
       </c>
-      <c r="BL209" s="1">
+      <c r="BL210" s="1">
         <v>44838</v>
       </c>
-      <c r="BM209" t="str">
+      <c r="BM210" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
-      <c r="BO209" s="1">
+      <c r="BO210" s="1">
         <v>44936</v>
       </c>
-      <c r="BR209" s="1">
+      <c r="BR210" s="1">
         <v>44968</v>
       </c>
-      <c r="BS209" s="1">
+      <c r="BS210" s="1">
         <v>44962</v>
       </c>
-      <c r="BT209" s="1">
+      <c r="BT210" s="1">
         <v>44962</v>
       </c>
-      <c r="BU209" t="str">
+      <c r="BU210" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
-      <c r="BW209" s="1">
+      <c r="BW210" s="1">
         <v>44967</v>
       </c>
-      <c r="BX209" s="1">
+      <c r="BX210" s="1">
         <v>44967</v>
       </c>
-      <c r="BY209" s="1">
+      <c r="BY210" s="1">
         <v>44970</v>
       </c>
-      <c r="BZ209" s="1">
+      <c r="BZ210" s="1">
         <v>44972</v>
       </c>
-      <c r="CA209" s="1">
+      <c r="CA210" s="1">
         <v>44971</v>
       </c>
-      <c r="CB209" s="1">
+      <c r="CB210" s="1">
         <v>44972</v>
       </c>
-      <c r="CD209" s="1">
+      <c r="CD210" s="1">
         <v>44991</v>
       </c>
-      <c r="CE209" t="str">
+      <c r="CE210" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CF209" s="1">
+      <c r="CF210" s="1">
         <v>44995</v>
       </c>
-      <c r="CG209" s="1">
+      <c r="CG210" s="1">
         <v>44981</v>
       </c>
-      <c r="CH209" t="str">
+      <c r="CH210" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CI209" s="1">
+      <c r="CI210" s="1">
         <v>44986</v>
       </c>
-      <c r="CJ209">
+      <c r="CJ210">
         <v>20701905</v>
       </c>
-      <c r="CK209" s="1">
+      <c r="CK210" s="1">
         <v>44977</v>
       </c>
-      <c r="CL209" s="1">
+      <c r="CL210" s="1">
         <v>44972</v>
       </c>
-      <c r="CP209" t="str">
+      <c r="CP210" t="str">
         <v>Aprobada</v>
       </c>
-      <c r="CQ209" s="1">
+      <c r="CQ210" s="1">
         <v>44970</v>
       </c>
-      <c r="CR209" t="str">
+      <c r="CR210" t="str">
         <v>SI</v>
       </c>
-      <c r="CS209" t="str">
+      <c r="CS210" t="str">
         <v>3</v>
       </c>
-      <c r="CT209" t="str" xml:space="preserve">
+      <c r="CT210" t="str" xml:space="preserve">
         <v xml:space="preserve">[2022-07-26 16:54:49] (Mayra Martinez) Archivo Subido (Fecha Envio RNP - RNP): RNP RIS7002
 [2022-10-04 13:36:39] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2022-10-14 06:36:26] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE RECHAZADO: Validar azimut y tilt ya que no da cobertura al mayor centro poblado
@@ -37695,231 +38096,231 @@
 [2023-03-10 15:23:49] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: RIS7002 ATP TX SAT: Se observa Instalación OK, Pruebas TH 4Mb/2Mb RFC OK, Fotos, seriales de módulos y pruebas de saturación OK.
 </v>
       </c>
-      <c r="CU209" t="str" xml:space="preserve">
+      <c r="CU210" t="str" xml:space="preserve">
         <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/RIS7002/Instalacion_TX/ATP-TX_RIS7002_AXESS_06-03-2023.pdf
 http://190.145.9.251/ftpsti/TowerTrack/RIS7002/Instalacion_RF/ATP-RF_RIS7002_HUAWEI_20-02-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7002/OC/RNP_RIS7002_TOWER3_26-07-2022.xlsx
 </v>
       </c>
     </row>
-    <row r="210" xml:space="preserve">
-      <c r="A210" t="str">
+    <row r="211" xml:space="preserve">
+      <c r="A211" t="str">
         <v>RIS7003</v>
       </c>
-      <c r="B210">
+      <c r="B211">
         <v>2</v>
       </c>
-      <c r="C210" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D210" t="str">
+      <c r="C211" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D211" t="str">
         <v>DEFINITIVO</v>
       </c>
-      <c r="F210" t="str">
+      <c r="F211" t="str">
         <v>OCCIDENTE</v>
       </c>
-      <c r="G210" t="str">
+      <c r="G211" t="str">
         <v>Andina</v>
       </c>
-      <c r="H210">
+      <c r="H211">
         <v>6</v>
       </c>
-      <c r="I210" t="str">
+      <c r="I211" t="str">
         <v>Res. 333</v>
       </c>
-      <c r="J210" s="1">
+      <c r="J211" s="1">
         <v>44651</v>
       </c>
-      <c r="K210" t="str">
+      <c r="K211" t="str">
         <v>Huawei</v>
       </c>
-      <c r="L210" t="str">
+      <c r="L211" t="str">
         <v>Axess</v>
       </c>
-      <c r="M210" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N210">
+      <c r="M211" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N211">
         <v>7</v>
       </c>
-      <c r="O210" t="str">
+      <c r="O211" t="str">
         <v>7.Integración RAD II</v>
       </c>
-      <c r="P210" t="str">
+      <c r="P211" t="str">
         <v>F2-RAD-Integrado RAD II</v>
       </c>
-      <c r="S210" t="str">
+      <c r="S211" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
-      <c r="T210" t="str">
+      <c r="T211" t="str">
         <v>F4-TX-E2E 1 OK</v>
       </c>
-      <c r="W210" s="1">
+      <c r="W211" s="1">
         <v>44516</v>
       </c>
-      <c r="X210" s="1">
+      <c r="X211" s="1">
         <v>44519</v>
       </c>
-      <c r="Y210" s="1">
+      <c r="Y211" s="1">
         <v>44519</v>
       </c>
-      <c r="Z210" s="1">
+      <c r="Z211" s="1">
         <v>44519</v>
       </c>
-      <c r="AA210">
+      <c r="AA211">
         <v>49</v>
       </c>
-      <c r="AB210" s="1">
+      <c r="AB211" s="1">
         <v>44531</v>
       </c>
-      <c r="AD210" s="1">
+      <c r="AD211" s="1">
         <v>44531</v>
       </c>
-      <c r="AG210" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AI210" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AJ210">
+      <c r="AG211" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AI211" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ211">
         <v>20241225</v>
       </c>
-      <c r="AK210" s="1">
+      <c r="AK211" s="1">
         <v>44565</v>
       </c>
-      <c r="AL210" t="str">
+      <c r="AL211" t="str">
         <v>Definitiva</v>
       </c>
-      <c r="AM210" t="str">
+      <c r="AM211" t="str">
         <v>Satelital</v>
       </c>
-      <c r="AN210" t="str">
+      <c r="AN211" t="str">
         <v>Solo Carrier</v>
       </c>
-      <c r="AO210">
+      <c r="AO211">
         <v>1</v>
       </c>
-      <c r="AP210" t="str">
+      <c r="AP211" t="str">
         <v>RIS7003-SATELITAL</v>
       </c>
-      <c r="AR210" t="str">
+      <c r="AR211" t="str">
         <v>SATELITAL</v>
       </c>
-      <c r="AT210" t="str">
+      <c r="AT211" t="str">
         <v>Axesat</v>
       </c>
-      <c r="AU210">
+      <c r="AU211">
         <v>60882</v>
       </c>
-      <c r="AV210" s="1">
+      <c r="AV211" s="1">
         <v>44539</v>
       </c>
-      <c r="BA210" s="1">
+      <c r="BA211" s="1">
         <v>44567</v>
       </c>
-      <c r="BD210">
+      <c r="BD211">
         <v>9999999</v>
       </c>
-      <c r="BF210">
+      <c r="BF211">
         <v>20244935</v>
       </c>
-      <c r="BG210" s="1">
+      <c r="BG211" s="1">
         <v>44544</v>
       </c>
-      <c r="BH210">
+      <c r="BH211">
         <v>9999999</v>
       </c>
-      <c r="BJ210" s="1">
+      <c r="BJ211" s="1">
         <v>44545</v>
       </c>
-      <c r="BK210" s="1">
+      <c r="BK211" s="1">
         <v>44550</v>
       </c>
-      <c r="BL210" s="1">
+      <c r="BL211" s="1">
         <v>44545</v>
       </c>
-      <c r="BM210" t="str">
+      <c r="BM211" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
-      <c r="BO210" s="1">
+      <c r="BO211" s="1">
         <v>44532</v>
       </c>
-      <c r="BP210" s="1">
+      <c r="BP211" s="1">
         <v>44537</v>
       </c>
-      <c r="BQ210" s="1">
+      <c r="BQ211" s="1">
         <v>44546</v>
       </c>
-      <c r="BR210" s="1">
+      <c r="BR211" s="1">
         <v>44567</v>
       </c>
-      <c r="BS210" s="1">
+      <c r="BS211" s="1">
         <v>44567</v>
       </c>
-      <c r="BT210" s="1">
+      <c r="BT211" s="1">
         <v>44567</v>
       </c>
-      <c r="BU210" t="str">
+      <c r="BU211" t="str">
         <v>Pte subir evidencias de pruebas#， sitio instalado.</v>
       </c>
-      <c r="BW210" s="1">
+      <c r="BW211" s="1">
         <v>44588</v>
       </c>
-      <c r="BX210" s="1">
+      <c r="BX211" s="1">
         <v>44593</v>
       </c>
-      <c r="BY210" s="1">
+      <c r="BY211" s="1">
         <v>44595</v>
       </c>
-      <c r="BZ210" s="1">
+      <c r="BZ211" s="1">
         <v>44602</v>
       </c>
-      <c r="CA210" s="1">
+      <c r="CA211" s="1">
         <v>44602</v>
       </c>
-      <c r="CB210" s="1">
+      <c r="CB211" s="1">
         <v>44603</v>
       </c>
-      <c r="CD210" s="1">
+      <c r="CD211" s="1">
         <v>44584</v>
       </c>
-      <c r="CE210" t="str">
+      <c r="CE211" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CF210" s="1">
+      <c r="CF211" s="1">
         <v>44603</v>
       </c>
-      <c r="CG210" s="1">
+      <c r="CG211" s="1">
         <v>44694</v>
       </c>
-      <c r="CH210" t="str">
+      <c r="CH211" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CI210" s="1">
+      <c r="CI211" s="1">
         <v>44812</v>
       </c>
-      <c r="CJ210">
+      <c r="CJ211">
         <v>20345118</v>
       </c>
-      <c r="CK210" s="1">
+      <c r="CK211" s="1">
         <v>44635</v>
       </c>
-      <c r="CL210" s="1">
+      <c r="CL211" s="1">
         <v>44631</v>
       </c>
-      <c r="CP210" t="str">
+      <c r="CP211" t="str">
         <v>Aprobada</v>
       </c>
-      <c r="CQ210" s="1">
+      <c r="CQ211" s="1">
         <v>44585</v>
       </c>
-      <c r="CR210" t="str">
+      <c r="CR211" t="str">
         <v>SI</v>
       </c>
-      <c r="CS210" t="str">
+      <c r="CS211" t="str">
         <v>2</v>
       </c>
-      <c r="CT210" t="str" xml:space="preserve">
+      <c r="CT211" t="str" xml:space="preserve">
         <v xml:space="preserve">[2022-01-04 09:50:50] (TowerTrack) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2022-01-14 18:24:25] (Jonathan Madronero) Comentarios E2E 2: Pte subir evidencias de pruebas#， sitio instalado.
 [2022-01-23 22:58:53] (Juan Lozada) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Archivo Subido
@@ -37933,117 +38334,117 @@
 [2022-09-08 08:15:14] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: APROBADO CON PENDIENTES: VSWR ok, Sin ALARMAS , Cross Feeder OK, SERIALES, Fotos ok, , Parametros de configuración validados directamente desde U2020 en operación normal.
 </v>
       </c>
-      <c r="CU210" t="str" xml:space="preserve">
+      <c r="CU211" t="str" xml:space="preserve">
         <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/RIS7003/Instalacion_RF/ATP-RF_RIS7003_HUAWEI_13-05-2022_VersionFinal.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7003/Instalacion_RF/ATP-RF_RIS7003_HUAWEI_13-05-2022.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7003/Instalacion_TX/ATP-TX_RIS7003_AXESS_23-01-2022.pdf
 </v>
       </c>
     </row>
-    <row r="211">
-      <c r="A211" t="str">
+    <row r="212">
+      <c r="A212" t="str">
         <v>RIS7004</v>
       </c>
-      <c r="B211">
+      <c r="B212">
         <v>5</v>
       </c>
-      <c r="C211" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D211" t="str">
+      <c r="C212" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D212" t="str">
         <v>DEFINITIVO</v>
       </c>
-      <c r="F211" t="str">
+      <c r="F212" t="str">
         <v>OCCIDENTE</v>
       </c>
-      <c r="G211" t="str">
+      <c r="G212" t="str">
         <v>Andina</v>
       </c>
-      <c r="H211">
+      <c r="H212">
         <v>6</v>
       </c>
-      <c r="I211" t="str">
+      <c r="I212" t="str">
         <v>Res. 332</v>
       </c>
-      <c r="J211" s="1">
+      <c r="J212" s="1">
         <v>45781</v>
       </c>
-      <c r="K211" t="str">
+      <c r="K212" t="str">
         <v>Huawei</v>
       </c>
-      <c r="L211" t="str">
+      <c r="L212" t="str">
         <v>NEC</v>
       </c>
-      <c r="M211" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N211">
+      <c r="M212" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N212">
         <v>47</v>
       </c>
-      <c r="O211" t="str">
+      <c r="O212" t="str">
         <v>1.SAQ</v>
       </c>
-      <c r="P211" t="str">
+      <c r="P212" t="str">
         <v>F1-SAQ-Busqueda y Negociación</v>
       </c>
-      <c r="S211" t="str">
+      <c r="S212" t="str">
         <v>1.HLD</v>
       </c>
-      <c r="T211" t="str">
+      <c r="T212" t="str">
         <v>F0-HLD-No iniciado</v>
       </c>
-      <c r="X211" s="1">
+      <c r="X212" s="1">
         <v>45585</v>
       </c>
-      <c r="AA211">
+      <c r="AA212">
         <v>45</v>
       </c>
-      <c r="AB211" s="1">
+      <c r="AB212" s="1">
         <v>45605</v>
       </c>
-      <c r="AL211" t="str">
+      <c r="AL212" t="str">
         <v>Definitiva</v>
       </c>
-      <c r="AM211" t="str">
+      <c r="AM212" t="str">
         <v>MW</v>
       </c>
-      <c r="AO211">
+      <c r="AO212">
         <v>1</v>
       </c>
-      <c r="AP211" t="str">
+      <c r="AP212" t="str">
         <v>RIS7004-CHO0009</v>
       </c>
-      <c r="BR211" s="1">
+      <c r="BR212" s="1">
         <v>45612</v>
       </c>
-      <c r="BZ211" s="1">
+      <c r="BZ212" s="1">
         <v>45615</v>
       </c>
-      <c r="CE211" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="CH211" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="CP211" t="str">
+      <c r="CE212" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="CH212" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="CP212" t="str">
         <v>Sin Entregar</v>
       </c>
-      <c r="CR211" t="str">
+      <c r="CR212" t="str">
         <v>SI</v>
       </c>
-      <c r="CS211" t="str">
+      <c r="CS212" t="str">
         <v>5</v>
       </c>
-      <c r="CT211" t="str">
+      <c r="CT212" t="str">
         <v/>
       </c>
-      <c r="CU211" t="str">
+      <c r="CU212" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:CU211"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:CU212"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se creo un modulo para manejar la creación del directorio para guardar los archivos del scraping
</commit_message>
<xml_diff>
--- a/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
+++ b/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
@@ -12387,7 +12387,7 @@
         <v>7.Integración RAD II</v>
       </c>
       <c r="P64" t="str">
-        <v>F1-RAD-OC en ejecución</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S64" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -12535,6 +12535,9 @@
       </c>
       <c r="CK64" s="1">
         <v>45012</v>
+      </c>
+      <c r="CL64" s="1">
+        <v>45007</v>
       </c>
       <c r="CP64" t="str">
         <v>Aprobada</v>
@@ -17907,7 +17910,7 @@
         <v>45012</v>
       </c>
       <c r="CE90" t="str">
-        <v>En revision ESCO/STI</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CH90" t="str">
         <v>Pendiente vendor</v>
@@ -17928,6 +17931,7 @@
 [2023-03-01 09:48:29] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2023-03-16 14:22:59] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 [2023-03-27 10:02:11] (Juan Lozada) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Archivo Subido (Fecha Entrega ATP Tx - ATP Tx)
+[2023-03-29 07:52:20] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7079    ATP TX SAT:  Instalación OK, TH 4Mb/2Mb RFC OK, FOTOS OK, SERIES OK, SATUR OK
 </v>
       </c>
       <c r="CU90" t="str" xml:space="preserve">

</xml_diff>

<commit_message>
Se creo la rutina para dejar la última salida Output de análisis. Los escraping se crean de manera secuencial para que los procesos se produscan de manera correcta
</commit_message>
<xml_diff>
--- a/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
+++ b/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
@@ -1983,7 +1983,7 @@
         <v>14</v>
       </c>
       <c r="AB6" s="1">
-        <v>45015</v>
+        <v>45016</v>
       </c>
       <c r="AC6" s="1">
         <v>44991</v>
@@ -2159,10 +2159,10 @@
         <v>44957</v>
       </c>
       <c r="X7" s="1">
-        <v>45049</v>
+        <v>45055</v>
       </c>
       <c r="Y7" s="1">
-        <v>45049</v>
+        <v>45055</v>
       </c>
       <c r="AA7">
         <v>21</v>
@@ -2171,7 +2171,7 @@
         <v>45067</v>
       </c>
       <c r="AC7" s="1">
-        <v>45036</v>
+        <v>45050</v>
       </c>
       <c r="AL7" t="str">
         <v>Definitiva</v>
@@ -2179,11 +2179,23 @@
       <c r="AM7" t="str">
         <v>MW</v>
       </c>
+      <c r="AN7" t="str">
+        <v>Solo Carrier</v>
+      </c>
       <c r="AO7">
         <v>1</v>
       </c>
       <c r="AP7" t="str">
         <v>ANT7038-ANT1052</v>
+      </c>
+      <c r="AT7" t="str">
+        <v>EDATEL</v>
+      </c>
+      <c r="AU7">
+        <v>64566</v>
+      </c>
+      <c r="AV7" s="1">
+        <v>45008</v>
       </c>
       <c r="BR7" s="1">
         <v>45069</v>
@@ -4851,19 +4863,19 @@
         <v>44831</v>
       </c>
       <c r="X22" s="1">
-        <v>45031</v>
+        <v>45038</v>
       </c>
       <c r="Y22" s="1">
-        <v>45031</v>
+        <v>45038</v>
       </c>
       <c r="AA22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AB22" s="1">
-        <v>45035</v>
+        <v>45046</v>
       </c>
       <c r="AC22" s="1">
-        <v>45031</v>
+        <v>45038</v>
       </c>
       <c r="AF22" s="1">
         <v>44979</v>
@@ -17778,10 +17790,10 @@
         <v>14</v>
       </c>
       <c r="O90" t="str">
-        <v>6.ON AIR</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P90" t="str">
-        <v>F1-OA-ON AIR</v>
+        <v>F1-RAD-OC en ejecución</v>
       </c>
       <c r="S90" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -17914,6 +17926,12 @@
       </c>
       <c r="CH90" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ90">
+        <v>20731983</v>
+      </c>
+      <c r="CK90" s="1">
+        <v>45014</v>
       </c>
       <c r="CP90" t="str">
         <v>Sin Entregar</v>
@@ -18216,7 +18234,7 @@
         <v>4.Instalación Tx</v>
       </c>
       <c r="P92" t="str">
-        <v>F1-TX-En E2E 1</v>
+        <v>F5-TX-E2E 2 OK</v>
       </c>
       <c r="S92" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -18316,6 +18334,15 @@
       </c>
       <c r="BR92" s="1">
         <v>45012</v>
+      </c>
+      <c r="BS92" s="1">
+        <v>45014</v>
+      </c>
+      <c r="BT92" s="1">
+        <v>45014</v>
+      </c>
+      <c r="BU92" t="str">
+        <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
       <c r="BZ92" s="1">
         <v>45014</v>
@@ -18339,6 +18366,7 @@
         <v xml:space="preserve">[2023-02-28 08:54:55] (Jaime Meza) Archivo Subido (Fecha Envio RNP - RNP): version 1
 [2023-02-28 18:21:03] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design Opcion 1
 [2023-03-03 13:49:25] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
+[2023-03-29 13:03:54] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 </v>
       </c>
       <c r="CU92" t="str" xml:space="preserve">
@@ -34397,10 +34425,10 @@
         <v>14</v>
       </c>
       <c r="O179" t="str">
-        <v>4.Instalación Tx</v>
+        <v>6.ON AIR</v>
       </c>
       <c r="P179" t="str">
-        <v>F5-TX-E2E 2 OK</v>
+        <v>F1-OA-ON AIR</v>
       </c>
       <c r="S179" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -34492,7 +34520,22 @@
       <c r="BU179" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
+      <c r="BW179" s="1">
+        <v>45003</v>
+      </c>
+      <c r="BX179" s="1">
+        <v>45003</v>
+      </c>
+      <c r="BY179" s="1">
+        <v>45013</v>
+      </c>
       <c r="BZ179" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CA179" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CB179" s="1">
         <v>45014</v>
       </c>
       <c r="CE179" t="str">

</xml_diff>

<commit_message>
Se agregaron las rutas dinamicas para crear las carpetas por fuera del archivo empaquetado
</commit_message>
<xml_diff>
--- a/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
+++ b/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
@@ -2150,10 +2150,10 @@
         <v>F1-PW-En instalación</v>
       </c>
       <c r="S7" t="str">
-        <v>1.HLD</v>
+        <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
       <c r="T7" t="str">
-        <v>F0-HLD-No iniciado</v>
+        <v>F1-TX-Carrier OK / MSP pte</v>
       </c>
       <c r="W7" s="1">
         <v>44957</v>
@@ -2172,6 +2172,12 @@
       </c>
       <c r="AC7" s="1">
         <v>45050</v>
+      </c>
+      <c r="AJ7">
+        <v>20732106</v>
+      </c>
+      <c r="AK7" s="1">
+        <v>45014</v>
       </c>
       <c r="AL7" t="str">
         <v>Definitiva</v>

</xml_diff>

<commit_message>
Esta es la versión que funciona con el .exe fuera del comprimido .asar. Procedo a limpiar el código
</commit_message>
<xml_diff>
--- a/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
+++ b/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
@@ -1084,7 +1084,10 @@
         <v>44995</v>
       </c>
       <c r="CH2" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CI2" s="1">
+        <v>45014</v>
       </c>
       <c r="CJ2">
         <v>20710311</v>
@@ -1133,6 +1136,7 @@
 [2023-03-06 18:49:19] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO:  SOPORTE APROBADO: ANT7033 ATP TX: Se observan buenos niveles de RX OK, Se observa buena  Instalación OK, TH 88Mb/88Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 [2023-03-10 17:31:11] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
 [2023-03-13 10:56:26] (Yeison Cordoba) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: COVER OK, VSWR OK, CROSS FEEDER OK,ALARMAS SE VALIDAN OK, SERIALES OK, INSTALACION OK, MML OK, SVSTEST GRAF OK,
+[2023-03-29 16:42:40] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO:  SOPORTE APROBADO: Datos COVER OK, Medición VSWR OK, Prueba CROSS FEEDER OK, Sin ALARMAS, SERIALES OK, Se observa buena,  INSTALACION OK, Parámetros MML OK, SVSTEST GRAF OK,
 </v>
       </c>
       <c r="CU2" t="str" xml:space="preserve">
@@ -1983,7 +1987,7 @@
         <v>14</v>
       </c>
       <c r="AB6" s="1">
-        <v>45016</v>
+        <v>45018</v>
       </c>
       <c r="AC6" s="1">
         <v>44991</v>
@@ -2141,7 +2145,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O7" t="str">
         <v>3.Power</v>
@@ -2204,10 +2208,10 @@
         <v>45008</v>
       </c>
       <c r="BR7" s="1">
-        <v>45069</v>
+        <v>45074</v>
       </c>
       <c r="BZ7" s="1">
-        <v>45071</v>
+        <v>45077</v>
       </c>
       <c r="CE7" t="str">
         <v>Pendiente vendor</v>
@@ -2665,7 +2669,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N10">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="O10" t="str">
         <v>1.SAQ</v>
@@ -2701,10 +2705,10 @@
         <v>ANT7042-ANT7043:ANT7043-ANT0057</v>
       </c>
       <c r="BR10" s="1">
-        <v>45210</v>
+        <v>45678</v>
       </c>
       <c r="BZ10" s="1">
-        <v>45215</v>
+        <v>45681</v>
       </c>
       <c r="CE10" t="str">
         <v>Pendiente vendor</v>
@@ -4652,7 +4656,10 @@
         <v>44999</v>
       </c>
       <c r="CE20" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CF20" s="1">
+        <v>45014</v>
       </c>
       <c r="CG20" s="1">
         <v>44991</v>
@@ -4701,11 +4708,12 @@
 [2023-03-14 00:01:55] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacion 
 [2023-03-14 14:54:26] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: ANT7148    ATP TX: NIVELES OK, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 [2023-03-16 14:44:06] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI, Parametros validados mediante el MML Command
+[2023-03-29 17:12:01] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: ANT7148 ATP TX: NIVELES OK  Según Ingeniería, Se evidencia buena Instalación, Capacidad TH 42Mb/42Mb, pruebas  RFC OK, FOTOS OK, SERIES OK, Enlace en Operacion
 </v>
       </c>
       <c r="CU20" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/ANT7148/Instalacion_RF/ATP-RF_ANT7148_HUAWEI_06-03-2023.xlsx
-http://190.145.9.251/ftpsti/TowerTrack/ANT7148/Instalacion_TX/ATP-TX_ANT7148_NEC_14-03-2023.zip
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/ANT7148/Instalacion_TX/ATP-TX_ANT7148_NEC_14-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/ANT7148/Instalacion_RF/ATP-RF_ANT7148_HUAWEI_06-03-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7148/Tx/ANT7148_E2E-2_14-03-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7148/Tx/ANT7148_E2E-1_03-02-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/ANT7148/OC/RNP_ANT7148_TOWER3_13-01-2023.xlsx
@@ -4750,7 +4758,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N21">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="O21" t="str">
         <v>1.SAQ</v>
@@ -4786,10 +4794,10 @@
         <v>ANT7150-ANT7043:ANT7043-ANT0057</v>
       </c>
       <c r="BR21" s="1">
-        <v>45240</v>
+        <v>45160</v>
       </c>
       <c r="BZ21" s="1">
-        <v>45245</v>
+        <v>45163</v>
       </c>
       <c r="CE21" t="str">
         <v>Pendiente vendor</v>
@@ -4851,7 +4859,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O22" t="str">
         <v>5.Instalación RF</v>
@@ -4953,13 +4961,13 @@
         <v>READY. OC E2E 20690661</v>
       </c>
       <c r="BR22" s="1">
-        <v>45038</v>
+        <v>45047</v>
       </c>
       <c r="BW22" s="1">
         <v>45046</v>
       </c>
       <c r="BZ22" s="1">
-        <v>45040</v>
+        <v>45048</v>
       </c>
       <c r="CE22" t="str">
         <v>Pendiente vendor</v>
@@ -6574,10 +6582,10 @@
         <v>F1-PW-En instalación</v>
       </c>
       <c r="S31" t="str">
-        <v>1.HLD</v>
+        <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
       <c r="T31" t="str">
-        <v>F0-HLD-No iniciado</v>
+        <v>F1-TX-Carrier OK / MSP pte</v>
       </c>
       <c r="W31" s="1">
         <v>44802</v>
@@ -6595,13 +6603,19 @@
         <v>45056</v>
       </c>
       <c r="AC31" s="1">
-        <v>45043</v>
+        <v>45050</v>
       </c>
       <c r="AG31" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="AI31" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ31">
+        <v>20727426</v>
+      </c>
+      <c r="AK31" s="1">
+        <v>45014</v>
       </c>
       <c r="AL31" t="str">
         <v>Definitiva</v>
@@ -6614,6 +6628,18 @@
       </c>
       <c r="AP31" t="str">
         <v>CHO7011-CHO7041:CHO7041-ANT0073</v>
+      </c>
+      <c r="AR31" t="str">
+        <v>ANT0073</v>
+      </c>
+      <c r="AT31" t="str">
+        <v>EDATEL</v>
+      </c>
+      <c r="AU31">
+        <v>64565</v>
+      </c>
+      <c r="AV31" s="1">
+        <v>45008</v>
       </c>
       <c r="BR31" s="1">
         <v>45061</v>
@@ -6956,10 +6982,10 @@
         <v>CHO7013-SATELITAL</v>
       </c>
       <c r="BR33" s="1">
-        <v>45800</v>
+        <v>45802</v>
       </c>
       <c r="BZ33" s="1">
-        <v>45803</v>
+        <v>45805</v>
       </c>
       <c r="CE33" t="str">
         <v>Pendiente vendor</v>
@@ -7497,10 +7523,10 @@
         <v>44795</v>
       </c>
       <c r="X37" s="1">
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="Y37" s="1">
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="AA37">
         <v>23</v>
@@ -7509,7 +7535,7 @@
         <v>45080</v>
       </c>
       <c r="AC37" s="1">
-        <v>45061</v>
+        <v>45068</v>
       </c>
       <c r="AG37" t="str">
         <v>Pendiente vendor</v>
@@ -9929,10 +9955,10 @@
         <v>14</v>
       </c>
       <c r="O53" t="str">
-        <v>4.Instalación Tx</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P53" t="str">
-        <v>F5-TX-E2E 2 OK</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S53" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -10033,14 +10059,38 @@
       <c r="BU53" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
+      <c r="BW53" s="1">
+        <v>45014</v>
+      </c>
+      <c r="BX53" s="1">
+        <v>45010</v>
+      </c>
+      <c r="BY53" s="1">
+        <v>45014</v>
+      </c>
       <c r="BZ53" s="1">
         <v>45014</v>
       </c>
+      <c r="CA53" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CB53" s="1">
+        <v>45014</v>
+      </c>
       <c r="CE53" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="CH53" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ53">
+        <v>20732617</v>
+      </c>
+      <c r="CK53" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CL53" s="1">
+        <v>45014</v>
       </c>
       <c r="CP53" t="str">
         <v>Sin Entregar</v>
@@ -11499,8 +11549,11 @@
       <c r="CB59" s="1">
         <v>44997</v>
       </c>
+      <c r="CD59" s="1">
+        <v>45015</v>
+      </c>
       <c r="CE59" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CH59" t="str">
         <v>Pendiente vendor</v>
@@ -11532,10 +11585,15 @@
 [2022-12-11 16:29:49] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO
 [2023-03-06 09:47:33] (Luis Collazos) Comentarios E2E 2: NEC trabajando en punta B
 [2023-03-06 09:47:33] (Luis Collazos) Comentarios Generales: RF ya comisionado. Se integra RF con TX
+[2023-03-30 14:17:14] (Marilu Romero ) Archivo Subido (Fecha E2E 2 - Prueba E2E 2): SE ADJUNTA E2E
+[2023-03-30 14:31:14] (Marilu Romero ) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): se adjunta documentacion correspondiente
+[2023-03-31 08:40:07] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7041    ATP TX SD: NIVELES OK, Instalación OK, TH 180Mb/180Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 </v>
       </c>
       <c r="CU59" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7041/OC/RNP_CHO7041_TOWER3_25-08-2022.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7041/Instalacion_TX/ATP-TX_CHO7041_NEC_30-03-2023.zip
+http://190.145.9.251/ftpsti/TowerTrack/CHO7041/Tx/CHO7041_E2E-2_30-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7041/OC/RNP_CHO7041_TOWER3_25-08-2022.xlsx
 </v>
       </c>
     </row>
@@ -12318,7 +12376,10 @@
         <v>44998</v>
       </c>
       <c r="CH63" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CI63" s="1">
+        <v>45014</v>
       </c>
       <c r="CJ63">
         <v>20710311</v>
@@ -12352,11 +12413,12 @@
 [2023-03-13 10:38:43] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
 [2023-03-13 21:16:56] (Yeison Cordoba) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: COVER OK, VSWR OK, CROSS FEEDER OK,ALARMAS SE VALIDAN (MENOR), SERIALES OK, INSTALACION OK, MML OK, SVSTEST GRAF OK,
 [2023-03-16 14:27:40] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO:  SOPORTE APROBADO CON PENDIENTES: CHO7047 ATP TX SAT: Instalación OK, TH 4Mb/2Mb RFC OK, FOTOS OK, SERIES OK, SATUR OK. Sitio en Operacion.
+[2023-03-29 16:58:44] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: Datos COVER Incompletos, Medición VSWR OK, CROSS FEEDER OK, Validación ALARMAS  (MENOREs), SERIALES OK, Se observa buena  INSTALACION , Parámetros MML OK, SVSTEST GRAF OK,
 </v>
       </c>
       <c r="CU63" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7047/Instalacion_TX/ATP-TX_CHO7047_AXESS_06-03-2023.pdf
-http://190.145.9.251/ftpsti/TowerTrack/CHO7047/Instalacion_RF/ATP-RF_CHO7047_HUAWEI_13-03-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7047/Instalacion_RF/ATP-RF_CHO7047_HUAWEI_13-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7047/Instalacion_TX/ATP-TX_CHO7047_AXESS_06-03-2023.pdf
 http://190.145.9.251/ftpsti/TowerTrack/CHO7047/OC/RNP_CHO7047_TOWER3_20-01-2023.xlsx
 </v>
       </c>
@@ -12973,8 +13035,11 @@
       <c r="CE66" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="CG66" s="1">
+        <v>45015</v>
+      </c>
       <c r="CH66" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO/STI</v>
       </c>
       <c r="CJ66">
         <v>20729329</v>
@@ -13001,10 +13066,12 @@
 [2023-03-15 12:04:26] (Jaime Meza) Fecha Envio RNP - RNP: SOPORTE CORREGIDO: Se añade torre 48 mts (45 mts efectivos por soportería) Version 2
 [2023-03-15 12:16:32] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION 1 - Estructura de 48mts
 [2023-03-22 16:13:08] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
+[2023-03-30 16:16:39] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
 </v>
       </c>
       <c r="CU66" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7050/OC/RNP_CHO7050_TOWER3_28-02-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7050/Instalacion_RF/ATP-RF_CHO7050_HUAWEI_30-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7050/OC/RNP_CHO7050_TOWER3_28-02-2023.xlsx
 </v>
       </c>
     </row>
@@ -13049,10 +13116,10 @@
         <v>14</v>
       </c>
       <c r="O67" t="str">
-        <v>4.Instalación Tx</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P67" t="str">
-        <v>F5-TX-E2E 2 OK</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S67" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -13159,14 +13226,38 @@
       <c r="BU67" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
+      <c r="BW67" s="1">
+        <v>45010</v>
+      </c>
+      <c r="BX67" s="1">
+        <v>45010</v>
+      </c>
+      <c r="BY67" s="1">
+        <v>45013</v>
+      </c>
       <c r="BZ67" s="1">
         <v>45014</v>
       </c>
+      <c r="CA67" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CB67" s="1">
+        <v>45014</v>
+      </c>
       <c r="CE67" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="CH67" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ67">
+        <v>20732371</v>
+      </c>
+      <c r="CK67" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CL67" s="1">
+        <v>45014</v>
       </c>
       <c r="CP67" t="str">
         <v>Sin Entregar</v>
@@ -17799,7 +17890,7 @@
         <v>7.Integración RAD II</v>
       </c>
       <c r="P90" t="str">
-        <v>F1-RAD-OC en ejecución</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S90" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -17938,6 +18029,9 @@
       </c>
       <c r="CK90" s="1">
         <v>45014</v>
+      </c>
+      <c r="CL90" s="1">
+        <v>45013</v>
       </c>
       <c r="CP90" t="str">
         <v>Sin Entregar</v>
@@ -18237,10 +18331,10 @@
         <v>14</v>
       </c>
       <c r="O92" t="str">
-        <v>4.Instalación Tx</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P92" t="str">
-        <v>F5-TX-E2E 2 OK</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S92" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -18350,14 +18444,38 @@
       <c r="BU92" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
+      <c r="BW92" s="1">
+        <v>45010</v>
+      </c>
+      <c r="BX92" s="1">
+        <v>45010</v>
+      </c>
+      <c r="BY92" s="1">
+        <v>45014</v>
+      </c>
       <c r="BZ92" s="1">
         <v>45014</v>
       </c>
+      <c r="CA92" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CB92" s="1">
+        <v>45014</v>
+      </c>
       <c r="CE92" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="CH92" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ92">
+        <v>20732617</v>
+      </c>
+      <c r="CK92" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CL92" s="1">
+        <v>45014</v>
       </c>
       <c r="CP92" t="str">
         <v>Sin Entregar</v>
@@ -21226,7 +21344,10 @@
         <v>44998</v>
       </c>
       <c r="CE107" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CF107" s="1">
+        <v>45014</v>
       </c>
       <c r="CG107" s="1">
         <v>45006</v>
@@ -21266,11 +21387,12 @@
 [2023-03-14 14:26:16] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7098    ATP TX SAT:  Instalación OK, TH 4Mb/2Mb RFC OK, FOTOS OK, SERIES fotos borrosas, SATUR OK¡
 [2023-03-21 11:45:33] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
 [2023-03-22 09:57:40] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7098    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
+[2023-03-29 16:50:17] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: CHO7098 ATP TX SAT: Se observa Instalación OK, Capacidad TH 4Mb/2Mb Pruebas RFC OK, FOTOS OK, SERIES ok, Pruebas  SATUR OK. Enlace  en Servicio
 </v>
       </c>
       <c r="CU107" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7098/Instalacion_RF/ATP-RF_CHO7098_HUAWEI_21-03-2023.xlsx
-http://190.145.9.251/ftpsti/TowerTrack/CHO7098/Instalacion_TX/ATP-TX_CHO7098_AXESS_13-03-2023.pdf
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7098/Instalacion_TX/ATP-TX_CHO7098_AXESS_13-03-2023.pdf
+http://190.145.9.251/ftpsti/TowerTrack/CHO7098/Instalacion_RF/ATP-RF_CHO7098_HUAWEI_21-03-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/CHO7098/OC/RNP_CHO7098_TOWER3_21-02-2023.xlsx
 </v>
       </c>
@@ -21585,7 +21707,7 @@
         <v>44992</v>
       </c>
       <c r="X109" s="1">
-        <v>45179</v>
+        <v>45192</v>
       </c>
       <c r="AA109">
         <v>46</v>
@@ -22271,10 +22393,10 @@
         <v>Pendiente vendor</v>
       </c>
       <c r="AJ114">
-        <v>20512475</v>
+        <v>20732106</v>
       </c>
       <c r="AK114" s="1">
-        <v>44777</v>
+        <v>45014</v>
       </c>
       <c r="AL114" t="str">
         <v>Temporal</v>
@@ -22283,10 +22405,7 @@
         <v>Satelital</v>
       </c>
       <c r="AN114" t="str">
-        <v>Solo MW y/o IRU</v>
-      </c>
-      <c r="AO114">
-        <v>2</v>
+        <v>N/A</v>
       </c>
       <c r="AP114" t="str">
         <v>CHO7106(sat)-CHO7111:CHO7111-CHO0008</v>
@@ -22294,17 +22413,14 @@
       <c r="AQ114" t="str">
         <v>CHO7106</v>
       </c>
-      <c r="AR114" t="str">
-        <v>CHO0008</v>
-      </c>
       <c r="AT114" t="str">
         <v>Axesat</v>
       </c>
       <c r="AU114">
-        <v>63368</v>
+        <v>64578</v>
       </c>
       <c r="AV114" s="1">
-        <v>44777</v>
+        <v>45013</v>
       </c>
       <c r="BA114" s="1">
         <v>44545</v>
@@ -22579,7 +22695,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N116">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O116" t="str">
         <v>1.SAQ</v>
@@ -22621,10 +22737,10 @@
         <v>CHO7109-CHO0008</v>
       </c>
       <c r="BR116" s="1">
-        <v>45250</v>
+        <v>45265</v>
       </c>
       <c r="BZ116" s="1">
-        <v>45253</v>
+        <v>45268</v>
       </c>
       <c r="CE116" t="str">
         <v>Pendiente vendor</v>
@@ -22979,16 +23095,19 @@
         <v>45046</v>
       </c>
       <c r="Y119" s="1">
+        <v>45015</v>
+      </c>
+      <c r="Z119" s="1">
+        <v>45015</v>
+      </c>
+      <c r="AA119">
+        <v>18</v>
+      </c>
+      <c r="AB119" s="1">
         <v>45046</v>
       </c>
-      <c r="AA119">
-        <v>26</v>
-      </c>
-      <c r="AB119" s="1">
-        <v>45101</v>
-      </c>
       <c r="AC119" s="1">
-        <v>45046</v>
+        <v>45015</v>
       </c>
       <c r="AF119" s="1">
         <v>44979</v>
@@ -23879,7 +23998,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N126">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="O126" t="str">
         <v>1.SAQ</v>
@@ -23921,10 +24040,10 @@
         <v>CHO7122-CHO0008</v>
       </c>
       <c r="BR126" s="1">
-        <v>45148</v>
+        <v>45253</v>
       </c>
       <c r="BZ126" s="1">
-        <v>45151</v>
+        <v>45256</v>
       </c>
       <c r="CE126" t="str">
         <v>Pendiente vendor</v>
@@ -24580,7 +24699,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N130">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="O130" t="str">
         <v>3.Power</v>
@@ -24601,13 +24720,16 @@
         <v>45031</v>
       </c>
       <c r="Y130" s="1">
-        <v>45031</v>
+        <v>45015</v>
+      </c>
+      <c r="Z130" s="1">
+        <v>45015</v>
       </c>
       <c r="AA130">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AB130" s="1">
-        <v>45075</v>
+        <v>45039</v>
       </c>
       <c r="AC130" s="1">
         <v>45010</v>
@@ -24631,10 +24753,10 @@
         <v>CHO7128-CHO7132:CHO7132-CHO7143:CHO7143-CHO7144:CHO7144-CHO7146:CHO7146-CHO7147:CHO7147-VAC0090</v>
       </c>
       <c r="BR130" s="1">
-        <v>45080</v>
+        <v>45044</v>
       </c>
       <c r="BZ130" s="1">
-        <v>45083</v>
+        <v>45046</v>
       </c>
       <c r="CE130" t="str">
         <v>Pendiente vendor</v>
@@ -25314,7 +25436,7 @@
         <v>Huawei</v>
       </c>
       <c r="L134" t="str">
-        <v>Axess</v>
+        <v>NEC</v>
       </c>
       <c r="M134" t="str">
         <v>TOWER 3</v>
@@ -25332,7 +25454,7 @@
         <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
       <c r="T134" t="str">
-        <v>F4-TX-E2E 1 OK</v>
+        <v>F1-TX-Carrier OK / MSP pte</v>
       </c>
       <c r="W134" s="1">
         <v>44992</v>
@@ -25356,22 +25478,22 @@
         <v>Pendiente vendor</v>
       </c>
       <c r="AJ134">
-        <v>20704301</v>
+        <v>20733550</v>
       </c>
       <c r="AK134" s="1">
-        <v>44980</v>
+        <v>45015</v>
       </c>
       <c r="AL134" t="str">
         <v>Temporal</v>
       </c>
       <c r="AM134" t="str">
-        <v>Satelital</v>
+        <v>MW + Satelital</v>
       </c>
       <c r="AP134" t="str">
-        <v>CHO7132-SATELITAL</v>
+        <v>CHO7132-CHO7143;CHO7143-CHO7144</v>
       </c>
       <c r="AQ134" t="str">
-        <v>CHO7132</v>
+        <v>CHO7144</v>
       </c>
       <c r="AT134" t="str">
         <v>Axesat</v>
@@ -25381,24 +25503,6 @@
       </c>
       <c r="AV134" s="1">
         <v>44979</v>
-      </c>
-      <c r="BD134">
-        <v>9999999</v>
-      </c>
-      <c r="BF134">
-        <v>20709559</v>
-      </c>
-      <c r="BG134" s="1">
-        <v>44987</v>
-      </c>
-      <c r="BH134">
-        <v>9999999</v>
-      </c>
-      <c r="BJ134" s="1">
-        <v>44988</v>
-      </c>
-      <c r="BL134" s="1">
-        <v>44988</v>
       </c>
       <c r="BM134" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
@@ -29888,7 +29992,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N155">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="O155" t="str">
         <v>1.SAQ</v>
@@ -29930,10 +30034,10 @@
         <v>CHO7155-CHO7147:CHO7147-VAC0090</v>
       </c>
       <c r="BR155" s="1">
-        <v>45250</v>
+        <v>45346</v>
       </c>
       <c r="BZ155" s="1">
-        <v>45253</v>
+        <v>45349</v>
       </c>
       <c r="CE155" t="str">
         <v>Pendiente vendor</v>
@@ -31811,10 +31915,10 @@
         <v>F1-PW-En instalación</v>
       </c>
       <c r="S166" t="str">
-        <v>1.HLD</v>
+        <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
       <c r="T166" t="str">
-        <v>F0-HLD-No iniciado</v>
+        <v>F1-TX-Carrier OK / MSP pte</v>
       </c>
       <c r="W166" s="1">
         <v>44812</v>
@@ -31840,17 +31944,35 @@
       <c r="AI166" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="AJ166">
+        <v>20727426</v>
+      </c>
+      <c r="AK166" s="1">
+        <v>45014</v>
+      </c>
       <c r="AL166" t="str">
-        <v>Definitiva</v>
+        <v>Temporal</v>
       </c>
       <c r="AM166" t="str">
-        <v>MW</v>
+        <v>MW + Satelital</v>
       </c>
       <c r="AO166">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AP166" t="str">
-        <v>CHO7171-CHO7078:CHO7078-CHO7077:CHO7077-CHO7184:CHO7184-CHO7106:CHO7106-CHO7111:CHO7111-CHO0008</v>
+        <v>CHO7171-CHO7078:CHO7078-SATELITAL.Temp</v>
+      </c>
+      <c r="AQ166" t="str">
+        <v>CHO7078</v>
+      </c>
+      <c r="AT166" t="str">
+        <v>Axesat</v>
+      </c>
+      <c r="AU166">
+        <v>64564</v>
+      </c>
+      <c r="AV166" s="1">
+        <v>45008</v>
       </c>
       <c r="BR166" s="1">
         <v>45095</v>
@@ -33699,7 +33821,7 @@
         <v>Huawei</v>
       </c>
       <c r="L176" t="str">
-        <v>NEC</v>
+        <v>Axess</v>
       </c>
       <c r="M176" t="str">
         <v>TOWER 3</v>
@@ -33756,16 +33878,16 @@
         <v>Pendiente vendor</v>
       </c>
       <c r="AJ176">
-        <v>20643024</v>
+        <v>20732106</v>
       </c>
       <c r="AK176" s="1">
-        <v>45012</v>
+        <v>45014</v>
       </c>
       <c r="AL176" t="str">
         <v>Temporal</v>
       </c>
       <c r="AM176" t="str">
-        <v>MW + Satelital</v>
+        <v>Satelital</v>
       </c>
       <c r="AN176" t="str">
         <v>MW + Satelital</v>
@@ -33783,10 +33905,10 @@
         <v>Axesat</v>
       </c>
       <c r="AU176">
-        <v>64245</v>
+        <v>64578</v>
       </c>
       <c r="AV176" s="1">
-        <v>44902</v>
+        <v>45013</v>
       </c>
       <c r="BD176">
         <v>9999999</v>
@@ -34431,10 +34553,10 @@
         <v>14</v>
       </c>
       <c r="O179" t="str">
-        <v>6.ON AIR</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P179" t="str">
-        <v>F1-OA-ON AIR</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S179" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -34549,6 +34671,15 @@
       </c>
       <c r="CH179" t="str">
         <v>Pendiente vendor</v>
+      </c>
+      <c r="CJ179">
+        <v>20732243</v>
+      </c>
+      <c r="CK179" s="1">
+        <v>45014</v>
+      </c>
+      <c r="CL179" s="1">
+        <v>45014</v>
       </c>
       <c r="CP179" t="str">
         <v>Sin Entregar</v>
@@ -34832,10 +34963,10 @@
         <v>30</v>
       </c>
       <c r="O182" t="str">
-        <v>2.Civil Work</v>
+        <v>1.SAQ</v>
       </c>
       <c r="P182" t="str">
-        <v>F1-CW-En construcción</v>
+        <v>F2-SAQ-Contrato Firmado</v>
       </c>
       <c r="S182" t="str">
         <v>1.HLD</v>
@@ -34847,9 +34978,6 @@
         <v>44817</v>
       </c>
       <c r="X182" s="1">
-        <v>45107</v>
-      </c>
-      <c r="Y182" s="1">
         <v>45107</v>
       </c>
       <c r="AA182">
@@ -36084,7 +36212,7 @@
         <v>44802</v>
       </c>
       <c r="X193" s="1">
-        <v>45177</v>
+        <v>45192</v>
       </c>
       <c r="AA193">
         <v>46</v>
@@ -36522,7 +36650,7 @@
         <v>45013</v>
       </c>
       <c r="CE196" t="str">
-        <v>En revision ESCO/STI</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CG196" s="1">
         <v>45009</v>
@@ -36562,6 +36690,7 @@
 [2023-03-24 17:44:53] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión.  
 [2023-03-27 15:51:57] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7204    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS NA, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
 [2023-03-28 16:32:59] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacion paa revisión
+[2023-03-29 16:04:33] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7204    ATP TX: NIVELES OK, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 </v>
       </c>
       <c r="CU196" t="str" xml:space="preserve">
@@ -36621,7 +36750,7 @@
         <v>1.HLD</v>
       </c>
       <c r="T197" t="str">
-        <v>F0-HLD-No iniciado</v>
+        <v>F1-HLD-HLD OK</v>
       </c>
       <c r="W197" s="1">
         <v>44992</v>
@@ -36635,17 +36764,29 @@
       <c r="AB197" s="1">
         <v>45141</v>
       </c>
+      <c r="AJ197">
+        <v>20733550</v>
+      </c>
+      <c r="AK197" s="1">
+        <v>45015</v>
+      </c>
       <c r="AL197" t="str">
-        <v>Definitiva</v>
+        <v>Temporal</v>
       </c>
       <c r="AM197" t="str">
-        <v>MW</v>
+        <v>MW + Satelital</v>
       </c>
       <c r="AO197">
         <v>7</v>
       </c>
       <c r="AP197" t="str">
-        <v>CHO7205-CHO7128:CHO7128-CHO7132:CHO7132-CHO7143:CHO7143-CHO7144:CHO7144-CHO7146:CHO7146-CHO7147:CHO7147-VAC0090</v>
+        <v>CHO7205-CHO7132;CHO7132-CHO7143;CHO7143-CHO7144</v>
+      </c>
+      <c r="AQ197" t="str">
+        <v>CHO7144</v>
+      </c>
+      <c r="AT197" t="str">
+        <v>Axesat</v>
       </c>
       <c r="BR197" s="1">
         <v>45146</v>
@@ -37178,6 +37319,9 @@
       <c r="M203" t="str">
         <v>TOWER 3</v>
       </c>
+      <c r="N203">
+        <v>31</v>
+      </c>
       <c r="O203" t="str">
         <v>2.Civil Work</v>
       </c>
@@ -37201,6 +37345,12 @@
       </c>
       <c r="AB203" s="1">
         <v>45495</v>
+      </c>
+      <c r="BR203" s="1">
+        <v>45502</v>
+      </c>
+      <c r="BZ203" s="1">
+        <v>45505</v>
       </c>
       <c r="CE203" t="str">
         <v>Pendiente vendor</v>
@@ -37258,6 +37408,9 @@
       <c r="M204" t="str">
         <v>TOWER 3</v>
       </c>
+      <c r="N204">
+        <v>31</v>
+      </c>
       <c r="O204" t="str">
         <v>2.Civil Work</v>
       </c>
@@ -37281,6 +37434,12 @@
       </c>
       <c r="AB204" s="1">
         <v>45495</v>
+      </c>
+      <c r="BR204" s="1">
+        <v>45502</v>
+      </c>
+      <c r="BZ204" s="1">
+        <v>45505</v>
       </c>
       <c r="CE204" t="str">
         <v>Pendiente vendor</v>

</xml_diff>

<commit_message>
Se agregaron estilos y una función de pendiente cuando no hay datos que mostrar
</commit_message>
<xml_diff>
--- a/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
+++ b/public/00_Inputs/Sitios_Implementacion_TowerTrack.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CU212"/>
+  <dimension ref="A1:CU211"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -591,7 +591,6 @@
     <col min="208" max="208" width="20.83203125" customWidth="1"/>
     <col min="209" max="209" width="20.83203125" customWidth="1"/>
     <col min="210" max="210" width="20.83203125" customWidth="1"/>
-    <col min="211" max="211" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1340,10 +1339,10 @@
         <v>44986</v>
       </c>
       <c r="CH3" t="str">
-        <v>Aprobado con Pendientes</v>
+        <v>Aprobado</v>
       </c>
       <c r="CI3" s="1">
-        <v>44994</v>
+        <v>45016</v>
       </c>
       <c r="CJ3">
         <v>20701905</v>
@@ -1391,6 +1390,7 @@
 [2023-03-09 16:50:13] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO CON PENDIENTES: SOPORTE APROBADO CON PENDIENTES: ANT7034 ATP RF: Pendiente datos pagina COVER, Medición VSWR OK, Sin alarmas presentes, CROSS OK, Validacion de parametros mediante MML Command, SERIAL OK, INSTALACION OK.
 [2023-03-14 15:39:27] (Kevin Guerrero) Fecha Entrega ATP Rf - ATP RF: SOPORTE CORREGIDO: Anexo ATP nuevamente, el cover si esta completo. 
 [2023-03-14 16:37:01] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: ANT7034 ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: OK, 
+[2023-03-31 16:51:08] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO:  SOPORTE APROBADO:  ANT7034 ATP RF: Medición VSWR OK, Sin alarmas presentes, CROSS OK, Validacion de parametros mediante MML Command, SERIAL OK, INSTALACION OK. Sitio en Servicio
 </v>
       </c>
       <c r="CU3" t="str" xml:space="preserve">
@@ -1588,10 +1588,10 @@
         <v>44986</v>
       </c>
       <c r="CE4" t="str">
-        <v>Aprobado con Pendientes</v>
+        <v>Aprobado</v>
       </c>
       <c r="CF4" s="1">
-        <v>44995</v>
+        <v>45016</v>
       </c>
       <c r="CG4" s="1">
         <v>44991</v>
@@ -1652,6 +1652,7 @@
 [2023-03-16 14:39:28] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI. Sitio en Operacion.
 [2023-03-16 16:14:03] (Karla Lopez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE CORREGIDO: Se adjunta documentacion y pruebas RFC correcta.
 [2023-03-17 09:32:23] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: ANT7035 ATP TX: NIVELES OK, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK, ANEXAN: REPORTE RFC
+[2023-03-31 17:04:58] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: ANT7035 ATP TX: Se observa buenos niveles de RX, Instalación OK, TH 42Mb/42Mb RFC FALTA, FOTOS OK, SERIES OK, Personal OK, Se adjunta reporte de pruebas RFC
 </v>
       </c>
       <c r="CU4" t="str" xml:space="preserve">
@@ -1960,10 +1961,10 @@
         <v>15</v>
       </c>
       <c r="O6" t="str">
-        <v>3.Power</v>
+        <v>6.ON AIR</v>
       </c>
       <c r="P6" t="str">
-        <v>F1-PW-En instalación</v>
+        <v>F1-OA-ON AIR</v>
       </c>
       <c r="S6" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -1992,6 +1993,9 @@
       <c r="AC6" s="1">
         <v>44991</v>
       </c>
+      <c r="AD6" s="1">
+        <v>45018</v>
+      </c>
       <c r="AF6" s="1">
         <v>44998</v>
       </c>
@@ -2065,10 +2069,28 @@
         <v>READY. OC E2E 20711768</v>
       </c>
       <c r="BR6" s="1">
-        <v>45018</v>
+        <v>45024</v>
+      </c>
+      <c r="BU6" t="str">
+        <v>Pendiente punta A</v>
+      </c>
+      <c r="BW6" s="1">
+        <v>45020</v>
+      </c>
+      <c r="BX6" s="1">
+        <v>45020</v>
+      </c>
+      <c r="BY6" s="1">
+        <v>45025</v>
       </c>
       <c r="BZ6" s="1">
-        <v>45020</v>
+        <v>45024</v>
+      </c>
+      <c r="CA6" s="1">
+        <v>45025</v>
+      </c>
+      <c r="CB6" s="1">
+        <v>45025</v>
       </c>
       <c r="CE6" t="str">
         <v>Pendiente vendor</v>
@@ -2099,6 +2121,7 @@
 [2023-03-10 10:07:05] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE RECHAZADO: Se subió el mismo archivo de ANT7014
 [2023-03-13 11:34:08] (Jaime Meza) Fecha Envio RNP - RNP: SOPORTE CORREGIDO: Archivo correcto cargado V3
 [2023-03-15 15:09:23] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION 1
+[2023-04-03 10:11:03] (Luis Collazos) Comentarios E2E 2: Pendiente punta A
 </v>
       </c>
       <c r="CU6" t="str" xml:space="preserve">
@@ -2246,7 +2269,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D8" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F8" t="str">
         <v>OCCIDENTE</v>
@@ -2684,7 +2707,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X10" s="1">
-        <v>45657</v>
+        <v>46022</v>
       </c>
       <c r="AA10">
         <v>3</v>
@@ -2794,6 +2817,9 @@
         <v>45016</v>
       </c>
       <c r="Y11" s="1">
+        <v>45016</v>
+      </c>
+      <c r="Z11" s="1">
         <v>45016</v>
       </c>
       <c r="AA11">
@@ -2928,7 +2954,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D12" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F12" t="str">
         <v>OCCIDENTE</v>
@@ -3197,7 +3223,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O13" t="str">
         <v>4.Instalación Tx</v>
@@ -3308,13 +3334,13 @@
         <v>44928</v>
       </c>
       <c r="BR13" s="1">
-        <v>45018</v>
+        <v>45029</v>
       </c>
       <c r="BU13" t="str">
-        <v>sitio Vandalizado - Se espera recuperación en 9 días</v>
+        <v>NEC no ha podio ingresar a punta B. Se está cordinando acompañamiento</v>
       </c>
       <c r="BZ13" s="1">
-        <v>45018</v>
+        <v>45029</v>
       </c>
       <c r="CE13" t="str">
         <v>Pendiente vendor</v>
@@ -3344,6 +3370,8 @@
 [2023-02-05 21:10:03] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION 1
 [2023-02-24 14:20:05] (Luis Collazos) Comentarios E2E 2: sitio Vandalizado - Se espera recuperación en 9 días
 [2023-03-06 09:59:22] (Luis Collazos) Comentarios Generales: Se informa que TowerOne completará el sitio el 12 de marzo
+[2023-04-03 10:06:19] (Luis Collazos) Comentarios E2E 2: NEC no ha podio ingresar a punta B. Se está cordinando acompañamiento
+[2023-04-03 10:06:19] (Luis Collazos) Comentarios Generales: RF: instalado y comisionado
 </v>
       </c>
       <c r="CU13" t="str" xml:space="preserve">
@@ -3592,7 +3620,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O16" t="str">
         <v>4.Instalación Tx</v>
@@ -3712,13 +3740,13 @@
         <v>44977</v>
       </c>
       <c r="BR16" s="1">
-        <v>45018</v>
+        <v>45025</v>
       </c>
       <c r="BU16" t="str">
         <v>Paro Minero - NEC debe regresar a sitio</v>
       </c>
       <c r="BZ16" s="1">
-        <v>45018</v>
+        <v>45025</v>
       </c>
       <c r="CE16" t="str">
         <v>Pendiente vendor</v>
@@ -4039,13 +4067,13 @@
         <v>TOWER 3</v>
       </c>
       <c r="N18">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O18" t="str">
-        <v>5.Instalación RF</v>
+        <v>6.ON AIR</v>
       </c>
       <c r="P18" t="str">
-        <v>F3-RF-En transporte RF</v>
+        <v>F1-OA-ON AIR</v>
       </c>
       <c r="S18" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -4173,8 +4201,17 @@
       <c r="BX18" s="1">
         <v>44977</v>
       </c>
+      <c r="BY18" s="1">
+        <v>44981</v>
+      </c>
       <c r="BZ18" s="1">
-        <v>45018</v>
+        <v>45022</v>
+      </c>
+      <c r="CA18" s="1">
+        <v>45022</v>
+      </c>
+      <c r="CB18" s="1">
+        <v>45023</v>
       </c>
       <c r="CD18" s="1">
         <v>44992</v>
@@ -4211,6 +4248,7 @@
 [2023-03-07 12:30:09] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjunta documentacon correspondiente
 [2023-03-08 10:07:55] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: ANT7063    ATP TX: NIVELES OK, Instalación OK, TH 99Mb/99Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 [2023-03-22 15:20:05] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO:  SOPORTE APROBADO: ANT7063 ATP TX: NIVELES OK, Instalación OK, TH 99Mb/99Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
+[2023-04-03 10:11:51] (Luis Collazos) Comentarios Generales: RF regresaría el 05-04 a más tardar
 </v>
       </c>
       <c r="CU18" t="str" xml:space="preserve">
@@ -4877,10 +4915,10 @@
         <v>44831</v>
       </c>
       <c r="X22" s="1">
-        <v>45038</v>
+        <v>45044</v>
       </c>
       <c r="Y22" s="1">
-        <v>45038</v>
+        <v>45044</v>
       </c>
       <c r="AA22">
         <v>18</v>
@@ -4889,7 +4927,7 @@
         <v>45046</v>
       </c>
       <c r="AC22" s="1">
-        <v>45038</v>
+        <v>45044</v>
       </c>
       <c r="AF22" s="1">
         <v>44979</v>
@@ -6761,7 +6799,7 @@
         <v>44917</v>
       </c>
       <c r="AL32" t="str">
-        <v>Definitiva</v>
+        <v>Temporal</v>
       </c>
       <c r="AM32" t="str">
         <v>MW + Satelital</v>
@@ -8574,7 +8612,10 @@
         <v>45042</v>
       </c>
       <c r="Y45" s="1">
-        <v>45042</v>
+        <v>45019</v>
+      </c>
+      <c r="Z45" s="1">
+        <v>45019</v>
       </c>
       <c r="AA45">
         <v>20</v>
@@ -8583,7 +8624,7 @@
         <v>45056</v>
       </c>
       <c r="AC45" s="1">
-        <v>45029</v>
+        <v>45019</v>
       </c>
       <c r="AG45" t="str">
         <v>Pendiente vendor</v>
@@ -10093,7 +10134,7 @@
         <v>45014</v>
       </c>
       <c r="CP53" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR53" t="str">
         <v>SI</v>
@@ -11555,8 +11596,11 @@
       <c r="CE59" t="str">
         <v>En revision ESCO - (Aprobado STI)</v>
       </c>
+      <c r="CG59" s="1">
+        <v>45016</v>
+      </c>
       <c r="CH59" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CJ59">
         <v>20722643</v>
@@ -11588,10 +11632,13 @@
 [2023-03-30 14:17:14] (Marilu Romero ) Archivo Subido (Fecha E2E 2 - Prueba E2E 2): SE ADJUNTA E2E
 [2023-03-30 14:31:14] (Marilu Romero ) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): se adjunta documentacion correspondiente
 [2023-03-31 08:40:07] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7041    ATP TX SD: NIVELES OK, Instalación OK, TH 180Mb/180Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
+[2023-03-31 16:40:47] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
+[2023-04-03 10:17:03] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7041    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS NA, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
 </v>
       </c>
       <c r="CU59" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7041/Instalacion_TX/ATP-TX_CHO7041_NEC_30-03-2023.zip
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7041/Instalacion_RF/ATP-RF_CHO7041_HUAWEI_31-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7041/Instalacion_TX/ATP-TX_CHO7041_NEC_30-03-2023.zip
 http://190.145.9.251/ftpsti/TowerTrack/CHO7041/Tx/CHO7041_E2E-2_30-03-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/CHO7041/OC/RNP_CHO7041_TOWER3_25-08-2022.xlsx
 </v>
@@ -11845,7 +11892,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D61" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F61" t="str">
         <v>OCCIDENTE</v>
@@ -12607,8 +12654,11 @@
       <c r="CE64" t="str">
         <v>Pendiente vendor</v>
       </c>
+      <c r="CG64" s="1">
+        <v>45016</v>
+      </c>
       <c r="CH64" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CJ64">
         <v>20730161</v>
@@ -12638,10 +12688,13 @@
 [2023-02-22 17:57:33] (Jaime Meza) Fecha Envio RNP - RNP: SOPORTE CORREGIDO: Version 2
 [2023-02-23 14:41:56] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION  1
 [2023-03-13 08:31:13] (Luis Collazos) Comentarios E2E 2: Se inetraría RF con TX
+[2023-03-31 16:39:33] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
+[2023-04-03 09:56:37] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7048    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS NA, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
 </v>
       </c>
       <c r="CU64" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7048/OC/RNP_CHO7048_TOWER3_19-08-2022.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7048/Instalacion_RF/ATP-RF_CHO7048_HUAWEI_31-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7048/OC/RNP_CHO7048_TOWER3_19-08-2022.xlsx
 </v>
       </c>
     </row>
@@ -12821,7 +12874,10 @@
         <v>45006</v>
       </c>
       <c r="CH65" t="str">
-        <v>En revision ESCO - (Aprobado STI)</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CI65" s="1">
+        <v>45016</v>
       </c>
       <c r="CJ65">
         <v>20722643</v>
@@ -12858,6 +12914,7 @@
 [2023-03-13 09:02:30] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 [2023-03-21 11:44:16] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
 [2023-03-21 16:24:12] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7049    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS NA, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
+[2023-03-31 17:33:23] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: SOPORTE APROBADO: CHO7049 ATP RF: datos COVER OK, Medición y validación VSWR OK, sin alarmas  presentes, validación de parámetros de configuración mediante   MML Command OK, Seriales OK, INSTALACION OK, SVS TST: GRAF KPI
 </v>
       </c>
       <c r="CU65" t="str" xml:space="preserve">
@@ -13039,7 +13096,7 @@
         <v>45015</v>
       </c>
       <c r="CH66" t="str">
-        <v>En revision ESCO/STI</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CJ66">
         <v>20729329</v>
@@ -13051,7 +13108,7 @@
         <v>45009</v>
       </c>
       <c r="CP66" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR66" t="str">
         <v>SI</v>
@@ -13067,6 +13124,8 @@
 [2023-03-15 12:16:32] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION 1 - Estructura de 48mts
 [2023-03-22 16:13:08] (Juan Lozada) Comentarios E2E 2: Instalación Finalizada Pdte E2e y ATP
 [2023-03-30 16:16:39] (Kevin Guerrero) Archivo Subido (Fecha Entrega ATP Rf - ATP RF): Anexo ATP para revisión. 
+[2023-04-01 11:22:43] (Heber Mendez) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: CHO7050    ATP RF: COVER OK, VSWR OK, ALARM OK, CROSS OK, PARAM MML OK, SERIAL OK, INSTALACION OK, SVS TST: GRAF KPI
+NOTA: fotos de series demasiado alejadas, poco legibles, por favor mejorar.
 </v>
       </c>
       <c r="CU66" t="str" xml:space="preserve">
@@ -13260,7 +13319,7 @@
         <v>45014</v>
       </c>
       <c r="CP67" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR67" t="str">
         <v>SI</v>
@@ -17370,7 +17429,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D87" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F87" t="str">
         <v>OCCIDENTE</v>
@@ -18034,7 +18093,7 @@
         <v>45013</v>
       </c>
       <c r="CP90" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR90" t="str">
         <v>SI</v>
@@ -18349,10 +18408,10 @@
         <v>45006</v>
       </c>
       <c r="Y92" s="1">
-        <v>45053</v>
+        <v>45019</v>
       </c>
       <c r="Z92" s="1">
-        <v>45006</v>
+        <v>45019</v>
       </c>
       <c r="AA92">
         <v>13</v>
@@ -18361,7 +18420,7 @@
         <v>45011</v>
       </c>
       <c r="AC92" s="1">
-        <v>45048</v>
+        <v>45019</v>
       </c>
       <c r="AD92" s="1">
         <v>45011</v>
@@ -18478,7 +18537,7 @@
         <v>45014</v>
       </c>
       <c r="CP92" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR92" t="str">
         <v>SI</v>
@@ -18551,7 +18610,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X93" s="1">
-        <v>45303</v>
+        <v>45269</v>
       </c>
       <c r="AA93">
         <v>4</v>
@@ -19652,7 +19711,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D99" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F99" t="str">
         <v>OCCIDENTE</v>
@@ -20440,7 +20499,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X102" s="1">
-        <v>45442</v>
+        <v>45657</v>
       </c>
       <c r="AA102">
         <v>25</v>
@@ -20688,7 +20747,7 @@
         <v>45010</v>
       </c>
       <c r="CP103" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR103" t="str">
         <v>SI</v>
@@ -23068,19 +23127,19 @@
         <v>Huawei</v>
       </c>
       <c r="L119" t="str">
-        <v>Axess</v>
+        <v>NEC</v>
       </c>
       <c r="M119" t="str">
         <v>TOWER 3</v>
       </c>
       <c r="N119">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="O119" t="str">
-        <v>3.Power</v>
+        <v>4.Instalación Tx</v>
       </c>
       <c r="P119" t="str">
-        <v>F1-PW-En instalación</v>
+        <v>F1-TX-En E2E 1</v>
       </c>
       <c r="S119" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
@@ -23101,14 +23160,17 @@
         <v>45015</v>
       </c>
       <c r="AA119">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AB119" s="1">
-        <v>45046</v>
+        <v>45016</v>
       </c>
       <c r="AC119" s="1">
         <v>45015</v>
       </c>
+      <c r="AD119" s="1">
+        <v>45016</v>
+      </c>
       <c r="AF119" s="1">
         <v>44979</v>
       </c>
@@ -23128,7 +23190,7 @@
         <v>Temporal</v>
       </c>
       <c r="AM119" t="str">
-        <v>Satelital</v>
+        <v>MW + Satelital</v>
       </c>
       <c r="AN119" t="str">
         <v>MW + Satelital</v>
@@ -23173,10 +23235,10 @@
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
       <c r="BR119" s="1">
-        <v>45106</v>
+        <v>45030</v>
       </c>
       <c r="BZ119" s="1">
-        <v>45109</v>
+        <v>45032</v>
       </c>
       <c r="CE119" t="str">
         <v>Pendiente vendor</v>
@@ -24078,7 +24140,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D127" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F127" t="str">
         <v>OCCIDENTE</v>
@@ -24661,7 +24723,7 @@
 </v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" xml:space="preserve">
       <c r="A130" t="str">
         <v>CHO7128</v>
       </c>
@@ -24693,19 +24755,19 @@
         <v>Huawei</v>
       </c>
       <c r="L130" t="str">
-        <v>NEC</v>
+        <v>Axess</v>
       </c>
       <c r="M130" t="str">
         <v>TOWER 3</v>
       </c>
       <c r="N130">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O130" t="str">
-        <v>3.Power</v>
+        <v>4.Instalación Tx</v>
       </c>
       <c r="P130" t="str">
-        <v>F1-PW-En instalación</v>
+        <v>F1-TX-En E2E 1</v>
       </c>
       <c r="S130" t="str">
         <v>1.HLD</v>
@@ -24726,25 +24788,31 @@
         <v>45015</v>
       </c>
       <c r="AA130">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AB130" s="1">
-        <v>45039</v>
+        <v>45019</v>
       </c>
       <c r="AC130" s="1">
         <v>45010</v>
       </c>
+      <c r="AD130" s="1">
+        <v>45019</v>
+      </c>
+      <c r="AF130" s="1">
+        <v>45020</v>
+      </c>
       <c r="AG130" t="str">
-        <v>Pendiente vendor</v>
+        <v>RNP OK</v>
       </c>
       <c r="AI130" t="str">
         <v>Pendiente vendor</v>
       </c>
       <c r="AL130" t="str">
-        <v>Definitiva</v>
+        <v>Temporal</v>
       </c>
       <c r="AM130" t="str">
-        <v>MW</v>
+        <v>Satelital</v>
       </c>
       <c r="AO130">
         <v>6</v>
@@ -24752,11 +24820,32 @@
       <c r="AP130" t="str">
         <v>CHO7128-CHO7132:CHO7132-CHO7143:CHO7143-CHO7144:CHO7144-CHO7146:CHO7146-CHO7147:CHO7147-VAC0090</v>
       </c>
+      <c r="AT130" t="str">
+        <v>Axesat</v>
+      </c>
+      <c r="BD130">
+        <v>9999999</v>
+      </c>
+      <c r="BF130">
+        <v>9999999</v>
+      </c>
+      <c r="BH130">
+        <v>9999999</v>
+      </c>
+      <c r="BJ130" s="1">
+        <v>45016</v>
+      </c>
+      <c r="BL130" s="1">
+        <v>45016</v>
+      </c>
+      <c r="BM130" t="str">
+        <v>READY. Satelital</v>
+      </c>
       <c r="BR130" s="1">
         <v>45044</v>
       </c>
       <c r="BZ130" s="1">
-        <v>45046</v>
+        <v>45047</v>
       </c>
       <c r="CE130" t="str">
         <v>Pendiente vendor</v>
@@ -24773,11 +24862,15 @@
       <c r="CS130" t="str">
         <v>3</v>
       </c>
-      <c r="CT130" t="str">
-        <v/>
-      </c>
-      <c r="CU130" t="str">
-        <v/>
+      <c r="CT130" t="str" xml:space="preserve">
+        <v xml:space="preserve">[2023-04-03 09:44:01] (Sandra Galan) Comentarios E2E 1: READY. Satelital
+[2023-04-04 10:58:31] (Jaime Meza) Archivo Subido (Fecha Envio RNP - RNP): Version 1
+[2023-04-08 18:19:42] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design Opcion 1
+</v>
+      </c>
+      <c r="CU130" t="str" xml:space="preserve">
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7128/OC/RNP_CHO7128_TOWER3_04-04-2023.xlsx
+</v>
       </c>
     </row>
     <row r="131" xml:space="preserve">
@@ -25251,19 +25344,16 @@
         <v>20235245</v>
       </c>
       <c r="AL133" t="str">
-        <v>Temporal</v>
+        <v>Definitiva</v>
       </c>
       <c r="AM133" t="str">
         <v>Satelital</v>
       </c>
       <c r="AN133" t="str">
-        <v>Solo MW y/o IRU</v>
+        <v>Solo Carrier</v>
       </c>
       <c r="AO133">
         <v>4</v>
-      </c>
-      <c r="AP133" t="str">
-        <v>CHO7131-CHO7132:CHO7132-CHO7150:CHO7150-CHO7149:CHO7149-CHO7153:CHO7153-CHO7148:CHO7148-CHO7147:CHO7147-VAC0090</v>
       </c>
       <c r="AR133" t="str">
         <v>SATELITAL</v>
@@ -25815,7 +25905,7 @@
         <v>Huawei</v>
       </c>
       <c r="L136" t="str">
-        <v>NEC</v>
+        <v>Axess</v>
       </c>
       <c r="M136" t="str">
         <v>TOWER 3</v>
@@ -25871,20 +25961,20 @@
       <c r="AJ136">
         <v>20452208</v>
       </c>
+      <c r="AK136" s="1">
+        <v>45021</v>
+      </c>
       <c r="AL136" t="str">
         <v>Temporal</v>
       </c>
       <c r="AM136" t="str">
-        <v>MW + Satelital</v>
-      </c>
-      <c r="AN136" t="str">
-        <v>Solo Carrier</v>
+        <v>Satelital</v>
       </c>
       <c r="AO136">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AP136" t="str">
-        <v>CHO7134-CHO7133satelital TEMP)</v>
+        <v>CHO7134-CHO7133(Satelital TEMP)</v>
       </c>
       <c r="AQ136" t="str">
         <v>CHO7133</v>
@@ -26063,7 +26153,7 @@
         <v>Huawei</v>
       </c>
       <c r="L137" t="str">
-        <v>NEC</v>
+        <v>Por definir</v>
       </c>
       <c r="M137" t="str">
         <v>TOWER 3</v>
@@ -26098,17 +26188,8 @@
       <c r="AI137" t="str">
         <v>Pendiente vendor</v>
       </c>
-      <c r="AL137" t="str">
-        <v>Definitiva</v>
-      </c>
-      <c r="AM137" t="str">
-        <v>MW</v>
-      </c>
       <c r="AO137">
-        <v>2</v>
-      </c>
-      <c r="AP137" t="str">
-        <v>CHO7135-CHO7109:CHO7109-CHO0008</v>
+        <v>0</v>
       </c>
       <c r="BR137" s="1">
         <v>45582</v>
@@ -27740,7 +27821,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D145" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F145" t="str">
         <v>OCCIDENTE</v>
@@ -28597,7 +28678,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="D149" t="str">
-        <v>PLAN PISO</v>
+        <v>DEFINITIVO</v>
       </c>
       <c r="F149" t="str">
         <v>OCCIDENTE</v>
@@ -31833,8 +31914,11 @@
       <c r="CB165" s="1">
         <v>45008</v>
       </c>
+      <c r="CD165" s="1">
+        <v>45016</v>
+      </c>
       <c r="CE165" t="str">
-        <v>Pendiente vendor</v>
+        <v>En revision ESCO - (Aprobado STI)</v>
       </c>
       <c r="CH165" t="str">
         <v>Pendiente vendor</v>
@@ -31849,7 +31933,7 @@
         <v>45009</v>
       </c>
       <c r="CP165" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR165" t="str">
         <v>SI</v>
@@ -31861,10 +31945,15 @@
         <v xml:space="preserve">[2023-02-17 08:54:41] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2023-02-28 20:38:17] (Jaime Meza) Archivo Subido (Fecha Envio RNP - RNP): Version 1
 [2023-03-05 17:49:15] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE APROBADO: Aprobado New Design OPCION  1
+[2023-03-31 13:26:31] (Karla Lopez) Archivo Subido (Fecha E2E 2 - Prueba E2E 2): Se adjuta archiv de pruebas
+[2023-03-31 13:33:56] (Karla Lopez) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Se adjuta documentacion 
+[2023-04-03 09:40:24] (Heber Mendez) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: CHO7170    ATP TX: NIVELES OK, Instalación OK, TH 42Mb/42Mb RFC OK, FOTOS OK, SERIES OK, Personal OK
 </v>
       </c>
       <c r="CU165" t="str" xml:space="preserve">
-        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7170/OC/RNP_CHO7170_TOWER3_28-02-2023.xlsx
+        <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/CHO7170/Instalacion_TX/ATP-TX_CHO7170_NEC_31-03-2023.zip
+http://190.145.9.251/ftpsti/TowerTrack/CHO7170/Tx/CHO7170_E2E-2_31-03-2023.xlsx
+http://190.145.9.251/ftpsti/TowerTrack/CHO7170/OC/RNP_CHO7170_TOWER3_28-02-2023.xlsx
 </v>
       </c>
     </row>
@@ -34682,7 +34771,7 @@
         <v>45014</v>
       </c>
       <c r="CP179" t="str">
-        <v>Sin Entregar</v>
+        <v>En Revisión</v>
       </c>
       <c r="CR179" t="str">
         <v>SI</v>
@@ -37074,7 +37163,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X200" s="1">
-        <v>45807</v>
+        <v>45348</v>
       </c>
       <c r="AA200">
         <v>24</v>
@@ -37163,7 +37252,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X201" s="1">
-        <v>45309</v>
+        <v>45287</v>
       </c>
       <c r="AA201">
         <v>5</v>
@@ -37249,7 +37338,7 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X202" s="1">
-        <v>45344</v>
+        <v>45290</v>
       </c>
       <c r="AA202">
         <v>10</v>
@@ -37486,7 +37575,7 @@
         <v>Res. 333</v>
       </c>
       <c r="J205" s="1">
-        <v>44651</v>
+        <v>45016</v>
       </c>
       <c r="K205" t="str">
         <v>Huawei</v>
@@ -37672,7 +37761,7 @@
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>NEW7017</v>
+        <v>NEW7018</v>
       </c>
       <c r="B207">
         <v>5</v>
@@ -37708,7 +37797,7 @@
         <v>TOWER 3</v>
       </c>
       <c r="N207">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="O207" t="str">
         <v>1.SAQ</v>
@@ -37723,19 +37812,19 @@
         <v>F0-HLD-No iniciado</v>
       </c>
       <c r="X207" s="1">
-        <v>45585</v>
+        <v>45781</v>
       </c>
       <c r="AA207">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="AB207" s="1">
-        <v>45605</v>
+        <v>45795</v>
       </c>
       <c r="BR207" s="1">
-        <v>45612</v>
+        <v>45802</v>
       </c>
       <c r="BZ207" s="1">
-        <v>45615</v>
+        <v>45807</v>
       </c>
       <c r="CE207" t="str">
         <v>Pendiente vendor</v>
@@ -37759,12 +37848,12 @@
         <v/>
       </c>
     </row>
-    <row r="208">
+    <row r="208" xml:space="preserve">
       <c r="A208" t="str">
-        <v>NEW7018</v>
+        <v>RIS7001</v>
       </c>
       <c r="B208">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C208" t="str">
         <v>TOWER 3</v>
@@ -37785,278 +37874,189 @@
         <v>Res. 332</v>
       </c>
       <c r="J208" s="1">
-        <v>45781</v>
+        <v>45050</v>
       </c>
       <c r="K208" t="str">
         <v>Huawei</v>
       </c>
       <c r="L208" t="str">
-        <v>Por definir</v>
+        <v>Axess</v>
       </c>
       <c r="M208" t="str">
         <v>TOWER 3</v>
       </c>
       <c r="N208">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="O208" t="str">
-        <v>1.SAQ</v>
+        <v>7.Integración RAD II</v>
       </c>
       <c r="P208" t="str">
-        <v>F1-SAQ-Busqueda y Negociación</v>
+        <v>F2-RAD-Integrado RAD II</v>
       </c>
       <c r="S208" t="str">
-        <v>1.HLD</v>
+        <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
       <c r="T208" t="str">
-        <v>F0-HLD-No iniciado</v>
+        <v>F4-TX-E2E 1 OK</v>
+      </c>
+      <c r="W208" s="1">
+        <v>44729</v>
       </c>
       <c r="X208" s="1">
-        <v>45781</v>
+        <v>44822</v>
+      </c>
+      <c r="Y208" s="1">
+        <v>44822</v>
+      </c>
+      <c r="Z208" s="1">
+        <v>44822</v>
       </c>
       <c r="AA208">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="AB208" s="1">
-        <v>45795</v>
+        <v>44955</v>
+      </c>
+      <c r="AC208" s="1">
+        <v>44819</v>
+      </c>
+      <c r="AD208" s="1">
+        <v>44950</v>
+      </c>
+      <c r="AF208" s="1">
+        <v>44852</v>
+      </c>
+      <c r="AG208" t="str">
+        <v>RNP OK</v>
+      </c>
+      <c r="AI208" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ208">
+        <v>20533723</v>
+      </c>
+      <c r="AK208" s="1">
+        <v>44801</v>
+      </c>
+      <c r="AL208" t="str">
+        <v>Temporal</v>
+      </c>
+      <c r="AM208" t="str">
+        <v>Satelital</v>
+      </c>
+      <c r="AN208" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="AO208">
+        <v>0</v>
+      </c>
+      <c r="AP208" t="str">
+        <v>RIS7001-SATELITAL</v>
+      </c>
+      <c r="AT208" t="str">
+        <v>NA</v>
+      </c>
+      <c r="AU208">
+        <v>63502</v>
+      </c>
+      <c r="AV208" s="1">
+        <v>44798</v>
+      </c>
+      <c r="BD208">
+        <v>9999999</v>
+      </c>
+      <c r="BF208">
+        <v>20342350</v>
+      </c>
+      <c r="BG208" s="1">
+        <v>44270</v>
+      </c>
+      <c r="BH208">
+        <v>9999999</v>
+      </c>
+      <c r="BJ208" s="1">
+        <v>44838</v>
+      </c>
+      <c r="BL208" s="1">
+        <v>44838</v>
+      </c>
+      <c r="BM208" t="str">
+        <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
+      </c>
+      <c r="BO208" s="1">
+        <v>44936</v>
       </c>
       <c r="BR208" s="1">
-        <v>45802</v>
+        <v>44962</v>
+      </c>
+      <c r="BS208" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BT208" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BU208" t="str">
+        <v>Instalación Finalizada Pdte E2e y ATP</v>
+      </c>
+      <c r="BW208" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BX208" s="1">
+        <v>44963</v>
+      </c>
+      <c r="BY208" s="1">
+        <v>44965</v>
       </c>
       <c r="BZ208" s="1">
-        <v>45807</v>
+        <v>44967</v>
+      </c>
+      <c r="CA208" s="1">
+        <v>44967</v>
+      </c>
+      <c r="CB208" s="1">
+        <v>44967</v>
+      </c>
+      <c r="CD208" s="1">
+        <v>44971</v>
       </c>
       <c r="CE208" t="str">
-        <v>Pendiente vendor</v>
+        <v>Aprobado</v>
+      </c>
+      <c r="CF208" s="1">
+        <v>44974</v>
+      </c>
+      <c r="CG208" s="1">
+        <v>44977</v>
       </c>
       <c r="CH208" t="str">
-        <v>Pendiente vendor</v>
+        <v>Aprobado con Pendientes</v>
+      </c>
+      <c r="CI208" s="1">
+        <v>44991</v>
+      </c>
+      <c r="CJ208">
+        <v>20697685</v>
+      </c>
+      <c r="CK208" s="1">
+        <v>44971</v>
+      </c>
+      <c r="CL208" s="1">
+        <v>44971</v>
       </c>
       <c r="CP208" t="str">
-        <v>Sin Entregar</v>
+        <v>Aprobada</v>
+      </c>
+      <c r="CQ208" s="1">
+        <v>44970</v>
       </c>
       <c r="CR208" t="str">
         <v>SI</v>
       </c>
       <c r="CS208" t="str">
-        <v>5</v>
-      </c>
-      <c r="CT208" t="str">
-        <v/>
-      </c>
-      <c r="CU208" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="209" xml:space="preserve">
-      <c r="A209" t="str">
-        <v>RIS7001</v>
-      </c>
-      <c r="B209">
         <v>3</v>
       </c>
-      <c r="C209" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D209" t="str">
-        <v>DEFINITIVO</v>
-      </c>
-      <c r="F209" t="str">
-        <v>OCCIDENTE</v>
-      </c>
-      <c r="G209" t="str">
-        <v>Andina</v>
-      </c>
-      <c r="H209">
-        <v>6</v>
-      </c>
-      <c r="I209" t="str">
-        <v>Res. 332</v>
-      </c>
-      <c r="J209" s="1">
-        <v>45050</v>
-      </c>
-      <c r="K209" t="str">
-        <v>Huawei</v>
-      </c>
-      <c r="L209" t="str">
-        <v>Axess</v>
-      </c>
-      <c r="M209" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N209">
-        <v>7</v>
-      </c>
-      <c r="O209" t="str">
-        <v>7.Integración RAD II</v>
-      </c>
-      <c r="P209" t="str">
-        <v>F2-RAD-Integrado RAD II</v>
-      </c>
-      <c r="S209" t="str">
-        <v>2.Configuración TX (E2E 1-MSP)</v>
-      </c>
-      <c r="T209" t="str">
-        <v>F4-TX-E2E 1 OK</v>
-      </c>
-      <c r="W209" s="1">
-        <v>44729</v>
-      </c>
-      <c r="X209" s="1">
-        <v>44822</v>
-      </c>
-      <c r="Y209" s="1">
-        <v>44822</v>
-      </c>
-      <c r="Z209" s="1">
-        <v>44822</v>
-      </c>
-      <c r="AA209">
-        <v>5</v>
-      </c>
-      <c r="AB209" s="1">
-        <v>44955</v>
-      </c>
-      <c r="AC209" s="1">
-        <v>44819</v>
-      </c>
-      <c r="AD209" s="1">
-        <v>44950</v>
-      </c>
-      <c r="AF209" s="1">
-        <v>44852</v>
-      </c>
-      <c r="AG209" t="str">
-        <v>RNP OK</v>
-      </c>
-      <c r="AI209" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AJ209">
-        <v>20533723</v>
-      </c>
-      <c r="AK209" s="1">
-        <v>44801</v>
-      </c>
-      <c r="AL209" t="str">
-        <v>Temporal</v>
-      </c>
-      <c r="AM209" t="str">
-        <v>Satelital</v>
-      </c>
-      <c r="AN209" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="AO209">
-        <v>0</v>
-      </c>
-      <c r="AP209" t="str">
-        <v>RIS7001-SATELITAL</v>
-      </c>
-      <c r="AT209" t="str">
-        <v>NA</v>
-      </c>
-      <c r="AU209">
-        <v>63502</v>
-      </c>
-      <c r="AV209" s="1">
-        <v>44798</v>
-      </c>
-      <c r="BD209">
-        <v>9999999</v>
-      </c>
-      <c r="BF209">
-        <v>20342350</v>
-      </c>
-      <c r="BG209" s="1">
-        <v>44270</v>
-      </c>
-      <c r="BH209">
-        <v>9999999</v>
-      </c>
-      <c r="BJ209" s="1">
-        <v>44838</v>
-      </c>
-      <c r="BL209" s="1">
-        <v>44838</v>
-      </c>
-      <c r="BM209" t="str">
-        <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
-      </c>
-      <c r="BO209" s="1">
-        <v>44936</v>
-      </c>
-      <c r="BR209" s="1">
-        <v>44962</v>
-      </c>
-      <c r="BS209" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BT209" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BU209" t="str">
-        <v>Instalación Finalizada Pdte E2e y ATP</v>
-      </c>
-      <c r="BW209" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BX209" s="1">
-        <v>44963</v>
-      </c>
-      <c r="BY209" s="1">
-        <v>44965</v>
-      </c>
-      <c r="BZ209" s="1">
-        <v>44967</v>
-      </c>
-      <c r="CA209" s="1">
-        <v>44967</v>
-      </c>
-      <c r="CB209" s="1">
-        <v>44967</v>
-      </c>
-      <c r="CD209" s="1">
-        <v>44971</v>
-      </c>
-      <c r="CE209" t="str">
-        <v>Aprobado</v>
-      </c>
-      <c r="CF209" s="1">
-        <v>44974</v>
-      </c>
-      <c r="CG209" s="1">
-        <v>44977</v>
-      </c>
-      <c r="CH209" t="str">
-        <v>Aprobado con Pendientes</v>
-      </c>
-      <c r="CI209" s="1">
-        <v>44991</v>
-      </c>
-      <c r="CJ209">
-        <v>20697685</v>
-      </c>
-      <c r="CK209" s="1">
-        <v>44971</v>
-      </c>
-      <c r="CL209" s="1">
-        <v>44971</v>
-      </c>
-      <c r="CP209" t="str">
-        <v>Aprobada</v>
-      </c>
-      <c r="CQ209" s="1">
-        <v>44970</v>
-      </c>
-      <c r="CR209" t="str">
-        <v>SI</v>
-      </c>
-      <c r="CS209" t="str">
-        <v>3</v>
-      </c>
-      <c r="CT209" t="str" xml:space="preserve">
+      <c r="CT208" t="str" xml:space="preserve">
         <v xml:space="preserve">[2022-07-26 16:46:11] (Mayra Martinez) Archivo Subido (Fecha Envio RNP - RNP): RNP RIS7001
 [2022-10-04 13:35:27] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2022-10-14 06:32:19] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE RECHAZADO: Validar ajuste de azimuth y Tilt ya que no da cobertura sobre el mayor centro poblado
@@ -38073,222 +38073,222 @@
 [2023-03-06 17:26:05] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO CON PENDIENTES:  SOPORTE APROBADO CON PENDIENTES: Pestaña COVER OK, Medicion VSWR OK, Sin ALARM presentes, PARAM obtenidos mediante MML OK, SERIAL: antena 1 y 2 sin serial tigo, INSTALACION OK, Se observa muy poco trafico.
 </v>
       </c>
-      <c r="CU209" t="str" xml:space="preserve">
+      <c r="CU208" t="str" xml:space="preserve">
         <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/RIS7001/Instalacion_RF/ATP-RF_RIS7001_HUAWEI_20-02-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7001/Instalacion_TX/ATP-TX_RIS7001_AXESS_14-02-2023.pdf
 http://190.145.9.251/ftpsti/TowerTrack/RIS7001/OC/RNP_RIS7001_TOWER3_26-07-2022.xlsx
 </v>
       </c>
     </row>
-    <row r="210" xml:space="preserve">
-      <c r="A210" t="str">
+    <row r="209" xml:space="preserve">
+      <c r="A209" t="str">
         <v>RIS7002</v>
       </c>
-      <c r="B210">
+      <c r="B209">
         <v>3</v>
       </c>
-      <c r="C210" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D210" t="str">
+      <c r="C209" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D209" t="str">
         <v>DEFINITIVO</v>
       </c>
-      <c r="F210" t="str">
+      <c r="F209" t="str">
         <v>OCCIDENTE</v>
       </c>
-      <c r="G210" t="str">
+      <c r="G209" t="str">
         <v>Andina</v>
       </c>
-      <c r="H210">
+      <c r="H209">
         <v>6</v>
       </c>
-      <c r="I210" t="str">
+      <c r="I209" t="str">
         <v>Res. 332</v>
       </c>
-      <c r="J210" s="1">
+      <c r="J209" s="1">
         <v>45050</v>
       </c>
-      <c r="K210" t="str">
+      <c r="K209" t="str">
         <v>Huawei</v>
       </c>
-      <c r="L210" t="str">
+      <c r="L209" t="str">
         <v>Axess</v>
       </c>
-      <c r="M210" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N210">
+      <c r="M209" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N209">
         <v>8</v>
       </c>
-      <c r="O210" t="str">
+      <c r="O209" t="str">
         <v>7.Integración RAD II</v>
       </c>
-      <c r="P210" t="str">
+      <c r="P209" t="str">
         <v>F2-RAD-Integrado RAD II</v>
       </c>
-      <c r="S210" t="str">
+      <c r="S209" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
-      <c r="T210" t="str">
+      <c r="T209" t="str">
         <v>F4-TX-E2E 1 OK</v>
       </c>
-      <c r="W210" s="1">
+      <c r="W209" s="1">
         <v>44659</v>
       </c>
-      <c r="X210" s="1">
+      <c r="X209" s="1">
         <v>44802</v>
       </c>
-      <c r="Y210" s="1">
+      <c r="Y209" s="1">
         <v>44802</v>
       </c>
-      <c r="Z210" s="1">
+      <c r="Z209" s="1">
         <v>44802</v>
       </c>
-      <c r="AA210">
+      <c r="AA209">
         <v>6</v>
       </c>
-      <c r="AB210" s="1">
+      <c r="AB209" s="1">
         <v>44962</v>
       </c>
-      <c r="AC210" s="1">
+      <c r="AC209" s="1">
         <v>44799</v>
       </c>
-      <c r="AD210" s="1">
+      <c r="AD209" s="1">
         <v>44961</v>
       </c>
-      <c r="AF210" s="1">
+      <c r="AF209" s="1">
         <v>44852</v>
       </c>
-      <c r="AG210" t="str">
+      <c r="AG209" t="str">
         <v>RNP OK</v>
       </c>
-      <c r="AI210" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AJ210">
+      <c r="AI209" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ209">
         <v>20509315</v>
       </c>
-      <c r="AK210" s="1">
+      <c r="AK209" s="1">
         <v>44777</v>
       </c>
-      <c r="AL210" t="str">
+      <c r="AL209" t="str">
         <v>Definitiva</v>
       </c>
-      <c r="AM210" t="str">
+      <c r="AM209" t="str">
         <v>Satelital</v>
       </c>
-      <c r="AN210" t="str">
+      <c r="AN209" t="str">
         <v>N/A</v>
       </c>
-      <c r="AO210">
+      <c r="AO209">
         <v>0</v>
       </c>
-      <c r="AP210" t="str">
+      <c r="AP209" t="str">
         <v>RIS7002-SATELITAL</v>
       </c>
-      <c r="AT210" t="str">
+      <c r="AT209" t="str">
         <v>Axesat</v>
       </c>
-      <c r="AU210">
+      <c r="AU209">
         <v>63349</v>
       </c>
-      <c r="AV210" s="1">
+      <c r="AV209" s="1">
         <v>44775</v>
       </c>
-      <c r="BD210">
+      <c r="BD209">
         <v>9999999</v>
       </c>
-      <c r="BF210">
+      <c r="BF209">
         <v>20244935</v>
       </c>
-      <c r="BG210" s="1">
+      <c r="BG209" s="1">
         <v>44543</v>
       </c>
-      <c r="BH210">
+      <c r="BH209">
         <v>9999999</v>
       </c>
-      <c r="BJ210" s="1">
+      <c r="BJ209" s="1">
         <v>44838</v>
       </c>
-      <c r="BL210" s="1">
+      <c r="BL209" s="1">
         <v>44838</v>
       </c>
-      <c r="BM210" t="str">
+      <c r="BM209" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
-      <c r="BO210" s="1">
+      <c r="BO209" s="1">
         <v>44936</v>
       </c>
-      <c r="BR210" s="1">
+      <c r="BR209" s="1">
         <v>44968</v>
       </c>
-      <c r="BS210" s="1">
+      <c r="BS209" s="1">
         <v>44962</v>
       </c>
-      <c r="BT210" s="1">
+      <c r="BT209" s="1">
         <v>44962</v>
       </c>
-      <c r="BU210" t="str">
+      <c r="BU209" t="str">
         <v>Instalación Finalizada Pdte E2e y ATP</v>
       </c>
-      <c r="BW210" s="1">
+      <c r="BW209" s="1">
         <v>44967</v>
       </c>
-      <c r="BX210" s="1">
+      <c r="BX209" s="1">
         <v>44967</v>
       </c>
-      <c r="BY210" s="1">
+      <c r="BY209" s="1">
         <v>44970</v>
       </c>
-      <c r="BZ210" s="1">
+      <c r="BZ209" s="1">
         <v>44972</v>
       </c>
-      <c r="CA210" s="1">
+      <c r="CA209" s="1">
         <v>44971</v>
       </c>
-      <c r="CB210" s="1">
+      <c r="CB209" s="1">
         <v>44972</v>
       </c>
-      <c r="CD210" s="1">
+      <c r="CD209" s="1">
         <v>44991</v>
       </c>
-      <c r="CE210" t="str">
+      <c r="CE209" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CF210" s="1">
+      <c r="CF209" s="1">
         <v>44995</v>
       </c>
-      <c r="CG210" s="1">
+      <c r="CG209" s="1">
         <v>44981</v>
       </c>
-      <c r="CH210" t="str">
+      <c r="CH209" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CI210" s="1">
+      <c r="CI209" s="1">
         <v>44986</v>
       </c>
-      <c r="CJ210">
+      <c r="CJ209">
         <v>20701905</v>
       </c>
-      <c r="CK210" s="1">
+      <c r="CK209" s="1">
         <v>44977</v>
       </c>
-      <c r="CL210" s="1">
+      <c r="CL209" s="1">
         <v>44972</v>
       </c>
-      <c r="CP210" t="str">
+      <c r="CP209" t="str">
         <v>Aprobada</v>
       </c>
-      <c r="CQ210" s="1">
+      <c r="CQ209" s="1">
         <v>44970</v>
       </c>
-      <c r="CR210" t="str">
+      <c r="CR209" t="str">
         <v>SI</v>
       </c>
-      <c r="CS210" t="str">
+      <c r="CS209" t="str">
         <v>3</v>
       </c>
-      <c r="CT210" t="str" xml:space="preserve">
+      <c r="CT209" t="str" xml:space="preserve">
         <v xml:space="preserve">[2022-07-26 16:54:49] (Mayra Martinez) Archivo Subido (Fecha Envio RNP - RNP): RNP RIS7002
 [2022-10-04 13:36:39] (Sandra Galan) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2022-10-14 06:36:26] (Giovanni Lopez) Fecha Envio RNP - RNP: SOPORTE RECHAZADO: Validar azimut y tilt ya que no da cobertura al mayor centro poblado
@@ -38308,231 +38308,231 @@
 [2023-03-10 15:23:49] (Mario Roman) Fecha Entrega ATP Tx - ATP Tx: SOPORTE APROBADO: SOPORTE APROBADO: RIS7002 ATP TX SAT: Se observa Instalación OK, Pruebas TH 4Mb/2Mb RFC OK, Fotos, seriales de módulos y pruebas de saturación OK.
 </v>
       </c>
-      <c r="CU210" t="str" xml:space="preserve">
+      <c r="CU209" t="str" xml:space="preserve">
         <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/RIS7002/Instalacion_TX/ATP-TX_RIS7002_AXESS_06-03-2023.pdf
 http://190.145.9.251/ftpsti/TowerTrack/RIS7002/Instalacion_RF/ATP-RF_RIS7002_HUAWEI_20-02-2023.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7002/OC/RNP_RIS7002_TOWER3_26-07-2022.xlsx
 </v>
       </c>
     </row>
-    <row r="211" xml:space="preserve">
-      <c r="A211" t="str">
+    <row r="210" xml:space="preserve">
+      <c r="A210" t="str">
         <v>RIS7003</v>
       </c>
-      <c r="B211">
+      <c r="B210">
         <v>2</v>
       </c>
-      <c r="C211" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D211" t="str">
+      <c r="C210" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D210" t="str">
         <v>DEFINITIVO</v>
       </c>
-      <c r="F211" t="str">
+      <c r="F210" t="str">
         <v>OCCIDENTE</v>
       </c>
-      <c r="G211" t="str">
+      <c r="G210" t="str">
         <v>Andina</v>
       </c>
-      <c r="H211">
+      <c r="H210">
         <v>6</v>
       </c>
-      <c r="I211" t="str">
+      <c r="I210" t="str">
         <v>Res. 333</v>
       </c>
-      <c r="J211" s="1">
+      <c r="J210" s="1">
         <v>44651</v>
       </c>
-      <c r="K211" t="str">
+      <c r="K210" t="str">
         <v>Huawei</v>
       </c>
-      <c r="L211" t="str">
+      <c r="L210" t="str">
         <v>Axess</v>
       </c>
-      <c r="M211" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N211">
+      <c r="M210" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N210">
         <v>7</v>
       </c>
-      <c r="O211" t="str">
+      <c r="O210" t="str">
         <v>7.Integración RAD II</v>
       </c>
-      <c r="P211" t="str">
+      <c r="P210" t="str">
         <v>F2-RAD-Integrado RAD II</v>
       </c>
-      <c r="S211" t="str">
+      <c r="S210" t="str">
         <v>2.Configuración TX (E2E 1-MSP)</v>
       </c>
-      <c r="T211" t="str">
+      <c r="T210" t="str">
         <v>F4-TX-E2E 1 OK</v>
       </c>
-      <c r="W211" s="1">
+      <c r="W210" s="1">
         <v>44516</v>
       </c>
-      <c r="X211" s="1">
+      <c r="X210" s="1">
         <v>44519</v>
       </c>
-      <c r="Y211" s="1">
+      <c r="Y210" s="1">
         <v>44519</v>
       </c>
-      <c r="Z211" s="1">
+      <c r="Z210" s="1">
         <v>44519</v>
       </c>
-      <c r="AA211">
+      <c r="AA210">
         <v>49</v>
       </c>
-      <c r="AB211" s="1">
+      <c r="AB210" s="1">
         <v>44531</v>
       </c>
-      <c r="AD211" s="1">
+      <c r="AD210" s="1">
         <v>44531</v>
       </c>
-      <c r="AG211" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AI211" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="AJ211">
+      <c r="AG210" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AI210" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="AJ210">
         <v>20241225</v>
       </c>
-      <c r="AK211" s="1">
+      <c r="AK210" s="1">
         <v>44565</v>
       </c>
-      <c r="AL211" t="str">
+      <c r="AL210" t="str">
         <v>Definitiva</v>
       </c>
-      <c r="AM211" t="str">
+      <c r="AM210" t="str">
         <v>Satelital</v>
       </c>
-      <c r="AN211" t="str">
+      <c r="AN210" t="str">
         <v>Solo Carrier</v>
       </c>
-      <c r="AO211">
+      <c r="AO210">
         <v>1</v>
       </c>
-      <c r="AP211" t="str">
+      <c r="AP210" t="str">
         <v>RIS7003-SATELITAL</v>
       </c>
-      <c r="AR211" t="str">
+      <c r="AR210" t="str">
         <v>SATELITAL</v>
       </c>
-      <c r="AT211" t="str">
+      <c r="AT210" t="str">
         <v>Axesat</v>
       </c>
-      <c r="AU211">
+      <c r="AU210">
         <v>60882</v>
       </c>
-      <c r="AV211" s="1">
+      <c r="AV210" s="1">
         <v>44539</v>
       </c>
-      <c r="BA211" s="1">
+      <c r="BA210" s="1">
         <v>44567</v>
       </c>
-      <c r="BD211">
+      <c r="BD210">
         <v>9999999</v>
       </c>
-      <c r="BF211">
+      <c r="BF210">
         <v>20244935</v>
       </c>
-      <c r="BG211" s="1">
+      <c r="BG210" s="1">
         <v>44544</v>
       </c>
-      <c r="BH211">
+      <c r="BH210">
         <v>9999999</v>
       </c>
-      <c r="BJ211" s="1">
+      <c r="BJ210" s="1">
         <v>44545</v>
       </c>
-      <c r="BK211" s="1">
+      <c r="BK210" s="1">
         <v>44550</v>
       </c>
-      <c r="BL211" s="1">
+      <c r="BL210" s="1">
         <v>44545</v>
       </c>
-      <c r="BM211" t="str">
+      <c r="BM210" t="str">
         <v>READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP</v>
       </c>
-      <c r="BO211" s="1">
+      <c r="BO210" s="1">
         <v>44532</v>
       </c>
-      <c r="BP211" s="1">
+      <c r="BP210" s="1">
         <v>44537</v>
       </c>
-      <c r="BQ211" s="1">
+      <c r="BQ210" s="1">
         <v>44546</v>
       </c>
-      <c r="BR211" s="1">
+      <c r="BR210" s="1">
         <v>44567</v>
       </c>
-      <c r="BS211" s="1">
+      <c r="BS210" s="1">
         <v>44567</v>
       </c>
-      <c r="BT211" s="1">
+      <c r="BT210" s="1">
         <v>44567</v>
       </c>
-      <c r="BU211" t="str">
+      <c r="BU210" t="str">
         <v>Pte subir evidencias de pruebas#， sitio instalado.</v>
       </c>
-      <c r="BW211" s="1">
+      <c r="BW210" s="1">
         <v>44588</v>
       </c>
-      <c r="BX211" s="1">
+      <c r="BX210" s="1">
         <v>44593</v>
       </c>
-      <c r="BY211" s="1">
+      <c r="BY210" s="1">
         <v>44595</v>
       </c>
-      <c r="BZ211" s="1">
+      <c r="BZ210" s="1">
         <v>44602</v>
       </c>
-      <c r="CA211" s="1">
+      <c r="CA210" s="1">
         <v>44602</v>
       </c>
-      <c r="CB211" s="1">
+      <c r="CB210" s="1">
         <v>44603</v>
       </c>
-      <c r="CD211" s="1">
+      <c r="CD210" s="1">
         <v>44584</v>
       </c>
-      <c r="CE211" t="str">
+      <c r="CE210" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CF211" s="1">
+      <c r="CF210" s="1">
         <v>44603</v>
       </c>
-      <c r="CG211" s="1">
+      <c r="CG210" s="1">
         <v>44694</v>
       </c>
-      <c r="CH211" t="str">
+      <c r="CH210" t="str">
         <v>Aprobado</v>
       </c>
-      <c r="CI211" s="1">
+      <c r="CI210" s="1">
         <v>44812</v>
       </c>
-      <c r="CJ211">
+      <c r="CJ210">
         <v>20345118</v>
       </c>
-      <c r="CK211" s="1">
+      <c r="CK210" s="1">
         <v>44635</v>
       </c>
-      <c r="CL211" s="1">
+      <c r="CL210" s="1">
         <v>44631</v>
       </c>
-      <c r="CP211" t="str">
+      <c r="CP210" t="str">
         <v>Aprobada</v>
       </c>
-      <c r="CQ211" s="1">
+      <c r="CQ210" s="1">
         <v>44585</v>
       </c>
-      <c r="CR211" t="str">
+      <c r="CR210" t="str">
         <v>SI</v>
       </c>
-      <c r="CS211" t="str">
+      <c r="CS210" t="str">
         <v>2</v>
       </c>
-      <c r="CT211" t="str" xml:space="preserve">
+      <c r="CT210" t="str" xml:space="preserve">
         <v xml:space="preserve">[2022-01-04 09:50:50] (TowerTrack) Comentarios E2E 1: READY: Sitio Satelital se cierra con la configuracion de la OC de Datacom del MSP
 [2022-01-14 18:24:25] (Jonathan Madronero) Comentarios E2E 2: Pte subir evidencias de pruebas#， sitio instalado.
 [2022-01-23 22:58:53] (Juan Lozada) Archivo Subido (Fecha Entrega ATP Tx - ATP Tx): Archivo Subido
@@ -38546,117 +38546,117 @@
 [2022-09-08 08:15:14] (Mario Roman) Fecha Entrega ATP Rf - ATP RF: SOPORTE APROBADO: APROBADO CON PENDIENTES: VSWR ok, Sin ALARMAS , Cross Feeder OK, SERIALES, Fotos ok, , Parametros de configuración validados directamente desde U2020 en operación normal.
 </v>
       </c>
-      <c r="CU211" t="str" xml:space="preserve">
+      <c r="CU210" t="str" xml:space="preserve">
         <v xml:space="preserve">http://190.145.9.251/ftpsti/TowerTrack/RIS7003/Instalacion_RF/ATP-RF_RIS7003_HUAWEI_13-05-2022_VersionFinal.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7003/Instalacion_RF/ATP-RF_RIS7003_HUAWEI_13-05-2022.xlsx
 http://190.145.9.251/ftpsti/TowerTrack/RIS7003/Instalacion_TX/ATP-TX_RIS7003_AXESS_23-01-2022.pdf
 </v>
       </c>
     </row>
-    <row r="212">
-      <c r="A212" t="str">
+    <row r="211">
+      <c r="A211" t="str">
         <v>RIS7004</v>
       </c>
-      <c r="B212">
+      <c r="B211">
         <v>5</v>
       </c>
-      <c r="C212" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="D212" t="str">
+      <c r="C211" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="D211" t="str">
         <v>DEFINITIVO</v>
       </c>
-      <c r="F212" t="str">
+      <c r="F211" t="str">
         <v>OCCIDENTE</v>
       </c>
-      <c r="G212" t="str">
+      <c r="G211" t="str">
         <v>Andina</v>
       </c>
-      <c r="H212">
+      <c r="H211">
         <v>6</v>
       </c>
-      <c r="I212" t="str">
+      <c r="I211" t="str">
         <v>Res. 332</v>
       </c>
-      <c r="J212" s="1">
+      <c r="J211" s="1">
         <v>45781</v>
       </c>
-      <c r="K212" t="str">
+      <c r="K211" t="str">
         <v>Huawei</v>
       </c>
-      <c r="L212" t="str">
+      <c r="L211" t="str">
         <v>NEC</v>
       </c>
-      <c r="M212" t="str">
-        <v>TOWER 3</v>
-      </c>
-      <c r="N212">
+      <c r="M211" t="str">
+        <v>TOWER 3</v>
+      </c>
+      <c r="N211">
         <v>47</v>
       </c>
-      <c r="O212" t="str">
+      <c r="O211" t="str">
         <v>1.SAQ</v>
       </c>
-      <c r="P212" t="str">
+      <c r="P211" t="str">
         <v>F1-SAQ-Busqueda y Negociación</v>
       </c>
-      <c r="S212" t="str">
+      <c r="S211" t="str">
         <v>1.HLD</v>
       </c>
-      <c r="T212" t="str">
+      <c r="T211" t="str">
         <v>F0-HLD-No iniciado</v>
       </c>
-      <c r="X212" s="1">
+      <c r="X211" s="1">
         <v>45585</v>
       </c>
-      <c r="AA212">
+      <c r="AA211">
         <v>45</v>
       </c>
-      <c r="AB212" s="1">
+      <c r="AB211" s="1">
         <v>45605</v>
       </c>
-      <c r="AL212" t="str">
+      <c r="AL211" t="str">
         <v>Definitiva</v>
       </c>
-      <c r="AM212" t="str">
+      <c r="AM211" t="str">
         <v>MW</v>
       </c>
-      <c r="AO212">
+      <c r="AO211">
         <v>1</v>
       </c>
-      <c r="AP212" t="str">
+      <c r="AP211" t="str">
         <v>RIS7004-CHO0009</v>
       </c>
-      <c r="BR212" s="1">
+      <c r="BR211" s="1">
         <v>45612</v>
       </c>
-      <c r="BZ212" s="1">
+      <c r="BZ211" s="1">
         <v>45615</v>
       </c>
-      <c r="CE212" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="CH212" t="str">
-        <v>Pendiente vendor</v>
-      </c>
-      <c r="CP212" t="str">
+      <c r="CE211" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="CH211" t="str">
+        <v>Pendiente vendor</v>
+      </c>
+      <c r="CP211" t="str">
         <v>Sin Entregar</v>
       </c>
-      <c r="CR212" t="str">
+      <c r="CR211" t="str">
         <v>SI</v>
       </c>
-      <c r="CS212" t="str">
+      <c r="CS211" t="str">
         <v>5</v>
       </c>
-      <c r="CT212" t="str">
+      <c r="CT211" t="str">
         <v/>
       </c>
-      <c r="CU212" t="str">
+      <c r="CU211" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:CU212"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:CU211"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>